<commit_message>
Adding board for Geekworm WRover (8mb flash) model, preparing to get sound working
</commit_message>
<xml_diff>
--- a/wiring schematic.xlsx
+++ b/wiring schematic.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brobert\Documents\PlatformIO\Projects\ESP32-NES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brobert\Documents\code\esp32_nesemu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A26890-56BC-426D-8455-88D2CC547118}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA5FE2F-7FE8-4F72-8D7F-0DE22E1C8F48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13530" xr2:uid="{4F5E42A6-CAD7-4C07-9414-36130DA2E5E2}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>T_IRQ</t>
   </si>
@@ -100,6 +100,9 @@
   <si>
     <t>PS_CMD</t>
   </si>
+  <si>
+    <t>Speaker</t>
+  </si>
 </sst>
 </file>
 
@@ -136,7 +139,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -221,6 +224,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -234,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -251,6 +260,7 @@
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,8 +618,8 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="7238072" y="2676235"/>
-            <a:ext cx="104889" cy="90486"/>
+            <a:off x="7236485" y="2661418"/>
+            <a:ext cx="104889" cy="89428"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
@@ -673,8 +683,8 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="7266747" y="3438072"/>
-            <a:ext cx="106243" cy="112004"/>
+            <a:off x="7265160" y="3419022"/>
+            <a:ext cx="106243" cy="110946"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
@@ -973,15 +983,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>445544</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>44160</xdr:rowOff>
+      <xdr:colOff>431257</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>177510</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>531796</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>157942</xdr:rowOff>
+      <xdr:colOff>517509</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>110317</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
@@ -998,7 +1008,7 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="5119144" y="2592627"/>
+            <a:off x="5103270" y="1806285"/>
             <a:ext cx="86252" cy="113782"/>
           </xdr14:xfrm>
         </xdr:contentPart>
@@ -1683,6 +1693,885 @@
         </xdr:pic>
       </mc:Fallback>
     </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>361681</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>18785</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60035CF5-5227-4EC9-BFFD-14C8D32DCBDB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7415213" y="4953000"/>
+          <a:ext cx="2152381" cy="2123810"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>555419</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19174</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="42" name="Picture 41" descr="https://images-na.ssl-images-amazon.com/images/I/71RZLBxrdOL._SL1000_.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7A4497F-7B0E-45BD-97CC-B862C14FA211}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="4847" t="12378" r="5086" b="10758"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11039723" y="753960"/>
+          <a:ext cx="5595009" cy="4716111"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>217416</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>129318</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>341826</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>90565</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId46">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="43" name="Ink 42">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8B7BE0D-986C-42D9-96F7-A7DC3881E1FD}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="14579756" y="864104"/>
+            <a:ext cx="124410" cy="144944"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="8" name="Ink 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B99F8AB-9154-4508-824E-4BBBC1B8B00F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7071480" y="2443680"/>
+              <a:ext cx="147240" cy="160920"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>52622</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>168025</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>159242</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>72075</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId47">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="44" name="Ink 43">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5CB926D-A847-437B-86E3-D2977734E044}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="14414962" y="902811"/>
+            <a:ext cx="106620" cy="87747"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="9" name="Ink 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{939F5783-5173-46D7-B6B6-64BE6749FF9E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7084080" y="2658240"/>
+              <a:ext cx="128880" cy="105480"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>546662</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>154105</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>6566</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>84077</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId48">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="45" name="Ink 44">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0206F16-4FC4-4BE1-B2C6-5F91E659CCB5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="13616323" y="888891"/>
+            <a:ext cx="106243" cy="113669"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="10" name="Ink 9">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A6DA942-6B25-469D-B37C-4B5642079535}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7065131" y="3436395"/>
+              <a:ext cx="126000" cy="130538"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>327481</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>148950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>478491</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>91372</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId49">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="46" name="Ink 45">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{442AFCE1-5B11-458E-B4E5-E039B5CC5CD8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="13397142" y="883736"/>
+            <a:ext cx="151010" cy="126119"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="6" name="Ink 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B15A2331-F629-44C9-9648-3BF5E56E1FB6}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7075440" y="3650760"/>
+              <a:ext cx="168120" cy="145800"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>187708</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>137042</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>310679</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>74868</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId50">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="47" name="Ink 46">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A700410A-34C0-43B9-9FBF-7A9F334C3DCB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="11964691" y="871828"/>
+            <a:ext cx="122971" cy="121523"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="7" name="Ink 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CA364D8-7AD8-4366-B718-0778F6D16D6E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7066800" y="3849840"/>
+              <a:ext cx="145800" cy="136440"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>158662</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>144582</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>264336</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>103245</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId51">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="48" name="Ink 47">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45AE2CF0-CE76-4B52-A8C2-6D321EE4B338}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="13228323" y="879368"/>
+            <a:ext cx="105674" cy="142360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="4" name="Ink 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD656285-45B2-4A1F-87FC-06C94F22DDF5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7087320" y="4048200"/>
+              <a:ext cx="124920" cy="155160"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>451696</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>84418</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>537948</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>14503</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId52">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="49" name="Ink 48">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71A35580-E0BC-4ABE-AFDF-A589CC4C3EEF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="14814036" y="2656168"/>
+            <a:ext cx="86252" cy="113782"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="16" name="Ink 15">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8629E14D-C707-4B42-A3E1-FA1D74A1384F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7094520" y="2473560"/>
+              <a:ext cx="105480" cy="132480"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>60455</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>101450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>158541</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>38515</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId53">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="50" name="Ink 49">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55A4749D-64D5-441D-B2FE-641D00833C71}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="14422795" y="2673200"/>
+            <a:ext cx="98086" cy="120762"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="14" name="Ink 13">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49ACB3BF-9DF6-4658-99D2-18C5E9B64FCF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7087680" y="3049920"/>
+              <a:ext cx="116640" cy="142200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>514420</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>106401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>591820</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>20984</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId54">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="51" name="Ink 50">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C19263C5-3163-49BC-A725-28CDCE32F472}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="14230420" y="2678151"/>
+            <a:ext cx="77400" cy="98280"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="5" name="Ink 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28E5FDBA-F338-4041-ADB3-A7D19B6B13B7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5095440" y="2224080"/>
+              <a:ext cx="95040" cy="115920"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>304790</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>96704</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>396587</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>26047</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId55">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="52" name="Ink 51">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1994FAFE-FEC6-4706-963F-9EA3C81F377D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="14020790" y="2668454"/>
+            <a:ext cx="91797" cy="113040"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="11" name="Ink 10">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F0D0DA3-20B8-40C6-884E-0F4ADC6E9FC4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5096160" y="2400120"/>
+              <a:ext cx="113040" cy="130680"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>527693</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>98264</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>7926</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>34234</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId56">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="53" name="Ink 52">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{777C564B-1992-4542-80E5-1095197D67D8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="13597354" y="2670014"/>
+            <a:ext cx="126572" cy="119667"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="53" name="Ink 52">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{777C564B-1992-4542-80E5-1095197D67D8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId57"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13588466" y="2660921"/>
+              <a:ext cx="143993" cy="137490"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>414338</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>109538</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="54" name="Picture 53" descr="https://docs.platformio.org/en/latest/_images/espressif32_debug_pinout.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{157A9B48-7A1B-4A5C-87F3-51C321174299}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId58">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10915651" y="5472112"/>
+          <a:ext cx="15240000" cy="7629525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1882,7 +2771,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">28 132 5248,'-10'0'4565,"8"0"-2021,21-13 3125,44-7-5589,69 10 1733,-36 12-806,-74-3-5201,1 1-4981,-20 0 6962</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="801.854">6 200 6784,'0'0'169,"0"0"0,0 0 0,0 0 1,0-1-1,0 1 0,0 0 0,0 0 1,0 0-1,0 0 0,0-1 0,0 1 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 1,0-1-1,0 1 0,-1 0 0,1 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 1,-1-1-1,1 1 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,-1 0 0,1 0 0,0 0 1,0 0-1,0 1-169,0-21 2491,1 15-2371,1 0-1,-1 0 0,1 0 0,0 0 1,1 0-1,-1 0 0,1 1 0,0 0 1,0-1-1,1 1 0,-1 0 0,1 0 1,0 1-1,2-3-119,89-72 485,-66 55-266,-29 23-217,0 1 0,0-1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,0-1 0,0 1 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,-1 0 0,1 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0-1 1,0 1-1,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,1 0-2,-33 15 39,-28 23-116,52-31 69,1 1 0,1 0 0,0 0 0,0 1 0,0 0 0,1 0 0,1 0 0,-1 1 0,2-1 0,-1 1 8,4-6 22,-1-1-1,1 0 0,0 0 1,0 0-1,0 0 0,1 1 1,-1-1-1,1 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,1 0 0,-1-1 1,1 1-1,0 0 0,-1-1 1,1 1-1,1-1 0,-1 1 1,0-1-1,0 0 0,1 0 1,0 0-1,-1-1 0,1 1 1,0 0-1,0-1 0,-1 0 1,1 0-1,0 0 0,1 0 1,-1 0-1,0 0 0,0-1 1,0 0-22,50 5-27,-20-4-1922,-1 7-5755,-24-5 6691</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="801.853">6 200 6784,'0'0'169,"0"0"0,0 0 0,0 0 1,0-1-1,0 1 0,0 0 0,0 0 1,0 0-1,0 0 0,0-1 0,0 1 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 1,0-1-1,0 1 0,-1 0 0,1 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 1,-1-1-1,1 1 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,-1 0 0,1 0 0,0 0 1,0 0-1,0 1-169,0-21 2491,1 15-2371,1 0-1,-1 0 0,1 0 0,0 0 1,1 0-1,-1 0 0,1 1 0,0 0 1,0-1-1,1 1 0,-1 0 0,1 0 1,0 1-1,2-3-119,89-72 485,-66 55-266,-29 23-217,0 1 0,0-1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,0-1 0,0 1 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,-1 0 0,1 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0-1 1,0 1-1,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,1 0-2,-33 15 39,-28 23-116,52-31 69,1 1 0,1 0 0,0 0 0,0 1 0,0 0 0,1 0 0,1 0 0,-1 1 0,2-1 0,-1 1 8,4-6 22,-1-1-1,1 0 0,0 0 1,0 0-1,0 0 0,1 1 1,-1-1-1,1 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,1 0 0,-1-1 1,1 1-1,0 0 0,-1-1 1,1 1-1,1-1 0,-1 1 1,0-1-1,0 0 0,1 0 1,0 0-1,-1-1 0,1 1 1,0 0-1,0-1 0,-1 0 1,1 0-1,0 0 0,1 0 1,-1 0-1,0 0 0,0-1 1,0 0-22,50 5-27,-20-4-1922,-1 7-5755,-24-5 6691</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -1943,7 +2832,7 @@
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">191 19 3328,'6'-5'10290,"-6"-5"-6421,-24 11-2503,-14-5-678,5 8-203,26-1-442,6-3-39,0 0 0,-1 0 0,1 0-1,0 0 1,-1 0 0,1 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 1 0,0 0-1,0-1 1,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0-1,1 1 1,-1-1 0,1 0 0,-1 0 0,1 0 0,-1 2-4,17 35 37,39 60 139,-53-93-81,-1-1-1,0 0 0,0 0 0,0 1 0,0-1 0,-1 0 0,1 1 1,-1-1-1,0 0 0,-1 1 0,1-1 0,-1 1 0,0-1 1,0 0-1,0 0 0,-1 0 0,1 1 0,-1-1 0,0 0 1,0-1-1,0 1 0,-1 0 0,1-1 0,-1 1 0,0-1 0,0 0 1,0 0-1,-1 0 0,-3 2-94,4-2-148,-1 0-1,0-1 1,1 0 0,-1 0-1,0 0 1,0 0 0,-1-1 0,1 0-1,0 0 1,-1 0 0,1 0-1,-3 0 149,-14 0-4461,2-3-4444,14 1 6073</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="605.985">278 45 6656,'0'0'2144,"0"10"2618,-18 85-2189,14-61-5233,-2 0-4298,6-24 5113</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="874.835">220 51 6912,'5'12'7915,"6"-6"-4216,39-9-3708,-39 1 803,88-7-6415,-88 9 4955</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="874.834">220 51 6912,'5'12'7915,"6"-6"-4216,39-9-3708,-39 1 803,88-7-6415,-88 9 4955</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2090,6 +2979,230 @@
 </inkml:ink>
 </file>
 
+<file path=xl/ink/ink22.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-06-24T04:06:41.018"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#F6FFA3"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">118 343 5120,'3'-5'5022,"2"-10"-3882,-2 6-614,48-80 1911,-22 47-1782,-28 41-590,0-1 1,0 1-1,0 0 1,0 0-1,1 0 0,-1 0 1,0 0-1,0 0 1,1 0-1,-1 1 1,1-1-1,-1 0 1,0 1-1,1-1 1,-1 1-1,1 0 1,-1-1-1,1 1 0,0 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 1-1,1-1 1,-1 0-1,1 1 0,0 0-65,-1 1 90,1-1 0,-1 1 0,-1 0-1,1 0 1,0 0 0,0 0 0,-1 0-1,1 0 1,-1 0 0,1 0 0,-1 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,-1 0 0,0 0 0,1 0-1,-1 1-89,-1 0 118,1 0 1,0 0-1,-1 0 0,1 0 0,-1 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 0 0,-1 1 0,1-1 0,-1 0 0,0 0 0,1 0 0,-1-1 1,0 1-1,0-1 0,0 1 0,0-1 0,-1 0 0,1 0 0,0 0 0,0-1 0,-1 1 0,1-1 0,0 0 0,0 0 0,-2 0-118,3-2 25,-1 0-1,1-1 0,-1 1 0,1-1 1,0 0-1,0 1 0,0-1 0,1 0 0,-1 0 1,0 0-1,1 0 0,0-1 0,0 1 1,0 0-1,0-1 0,1 1 0,-1 0 1,1-1-1,0 1 0,0-1 0,0 1 1,0-2-25,0 2-6,0-1 1,0 0-1,0 1 1,0-1-1,1 1 1,-1-1-1,1 1 1,0-1-1,0 1 1,0-1-1,1 1 1,-1 0-1,1 0 1,0-1 0,-1 1-1,1 0 1,1 1-1,-1-1 1,0 0-1,1 1 1,0-1-1,-1 1 1,1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,1 1 1,-1-1-1,0 1 1,1 0-1,-1 0 1,1 0 0,-1 1-1,1-1 1,-1 1-1,1 0 1,1 0 5,52 16-310,-55-16 310,-1 1 0,1 0 0,-1-1-1,1 1 1,-1 0 0,0 0 0,0 0 0,1 0 0,-1 1 0,0-1-1,0 0 1,0 0 0,0 1 0,0-1 0,-1 0 0,1 1 0,0-1-1,-1 1 1,1-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,-1-1-1,0 1 1,0 0 0,0-1 0,0 1 0,0-1 0,-1 1 0,1 0-1,0-1 1,-1 1 0,1-1 0,-1 2 0,-3 4 11,-1 0 0,0-1 0,0 1 1,-1-1-1,1 0 0,-1-1 0,0 1 0,-1-1 0,1 0 0,-1-1 1,-5 3-12,6-4 6,1 1 1,-1-1-1,0-1 0,0 1 1,0-1-1,0 0 1,-1-1-1,1 1 1,0-1-1,-1 0 1,1-1-1,-2 1-6,6-1 3,-1-1 0,0 1 0,1 0 0,-1-1 1,1 1-1,-1-1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0-1 0,-1 1 1,1-1-1,0 1 0,0-1 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 1,-1 0-1,1-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 0-3,0 1-4,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0-1,-1 0 1,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0-1,-1 0 1,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,1 0-1,-1 1 1,0-1 0,1 1 0,0-1 0,-1 1 0,1 0 0,0 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0 0 0,0 0 0,0-1-1,0 1 1,1 0 0,-1 1 0,0-1 0,0 0 0,0 1 4,3 2-18,-1 0-1,1 1 1,-1-1 0,0 1-1,0 0 1,0 1 0,0-1-1,-1 1 1,1-1 0,-1 1-1,-1 0 1,1 0 0,-1 1-1,1-1 1,-1 0 0,-1 1 18,1 0 5,-1 0 1,1 0-1,-2 0 1,1 0-1,-1 0 1,1 0-1,-2 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,0-1-1,-1 1 1,0 0-1,0-1 1,-1 1-1,1-1 1,-1 1-1,0-1 1,-1 0-1,1 0 1,-1-1-1,0 1 1,0-1-1,-1 0 1,1 0-1,-1 0 0,0-1 1,0 1-1,0-1 1,0 0-1,-1-1 1,-3 2-6,5-4 11,1 0 0,-1-1-1,0 1 1,1-1 0,-1 0 0,1 0 0,-1 0 0,1 0-1,-1-1 1,1 1 0,0-1 0,0 0 0,0 0 0,0 0-1,0 0 1,0-1 0,0 1 0,1-1 0,-1 0 0,1 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,1-1-1,0 1 1,-1-1 0,1 1 0,1-1 0,-1 1-1,0-1 1,1-2-11,-3-5 1,2 0-1,-1 0 0,2 1 0,-1-1 1,2 0-1,-1 0 0,1 0 1,1 0-1,2-8 0,-3 16 0,-1-1 1,1 1-1,1-1 1,-1 1-1,0 0 0,1 0 1,0-1-1,0 1 1,0 0-1,0 0 1,0 1-1,0-1 1,1 0-1,-1 1 0,1-1 1,0 1-1,0 0 1,0 0-1,0 0 1,0 0-1,0 1 0,1-1 1,-1 1-1,0 0 1,1 0-1,-1 0 1,1 0-1,-1 1 0,1-1 1,0 1-1,0 0 0,3 0-19,0 0-1,0 1 1,-1 0-1,1 0 1,0 1-1,0-1 1,-1 2-1,1-1 1,-1 1 0,1 0-1,-1 0 1,0 0-1,0 1 1,-1 0-1,1 0 1,-1 1-1,0-1 1,0 1-1,0 1 1,-1-1-1,1 0 1,-1 1-1,0 1 20,-3-4 9,-1 0 0,1 0-1,-1 0 1,0 1 0,0-1-1,0 0 1,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0-1,0 0 1,0 0 0,0 0-1,-1 0 1,1-1 0,-1 1-1,1 0 1,-1-1 0,0 1-1,0-1 1,0 0 0,-1 1-1,1-1 1,0 0 0,-1 0-1,1-1 1,-1 1 0,0 0-1,1-1 1,-1 0 0,0 1-1,0-1 1,0-1 0,0 1-1,0 0 1,0-1 0,0 1-1,-1-1 1,1 0 0,0 0-1,0 0 1,0 0 0,0-1-1,0 1 1,0-1 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0-1 0,1 1-1,-1-1 1,1 0 0,-3-1-9,0-5 5,0 1 1,1-1 0,0 1 0,0-1 0,1 0-1,0 0 1,0-1 0,1 1 0,0-1 0,0 1-1,1-1 1,0 0 0,1 1 0,0-1 0,0 0-1,1 0 1,0 1 0,1-1 0,0 1 0,0-1-1,0 1 1,1-1 0,1 1-6,-3 5-2,0-1 1,0 1-1,0-1 1,1 1-1,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,1 0-1,-1 0 0,0 1 1,1-1-1,0 1 1,0 0-1,0-1 1,0 1-1,0 1 1,0-1-1,0 0 1,0 1-1,1 0 0,-1-1 1,1 2-1,-1-1 1,1 0-1,-1 0 1,1 1-1,0 0 1,-1 0-1,1 0 1,-1 0-1,1 1 1,0-1-1,-1 1 0,1 0 1,-1 0-1,2 1 2,4 2-48,0 1-1,0 1 0,-1 0 0,1 0 1,-1 1-1,0-1 0,-1 2 0,0-1 1,0 1-1,-1 0 0,5 9 49,-8-13-1,0 0 0,0 0 0,-1 1 0,1-1 0,-1 1 1,-1 0-1,1-1 0,-1 1 0,1 0 0,-1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 1 0,-1-1 0,1 0 0,-1 0 0,-1 0 0,1-1 0,-1 1 0,0 0 0,0 0 0,-1 0 1,1-1 21,-1-1-1,0 0 0,0 0 0,0 0 0,0-1 1,-1 1-1,1-1 0,-1 0 0,1 0 0,-1 0 1,0 0-1,0-1 0,0 1 0,0-1 1,0 0-1,0 0 0,0-1 0,0 1 0,0-1 1,0 0-1,0 0 0,-1 0 0,1 0 1,0-1-1,0 0 0,0 0 0,0 0 0,0 0 1,0-1-1,0 1 0,0-1 0,1 0 0,-1 0 1,1-1-1,-1 1 0,1-1 0,0 1 1,0-1-1,0 0 0,0 0 0,1-1 0,-1 1 1,-1-3-21,-1-2 1,0 0 0,1-1 1,0 1-1,0-1 0,1 0 1,0 0-1,1 0 0,0-1 1,0 1-1,1 0 0,0-1 1,1 1-1,0-1 0,0 1 1,1-1-1,0 1 0,1-1 1,0 1-1,1 0 0,0-1-1,-3 8-7,1 0 0,-1 0 0,1 0 0,0 0 0,-1 1-1,1-1 1,0 0 0,0 0 0,1 1 0,-1-1 0,0 1-1,0-1 1,1 1 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-1 0-1,1 0 1,0 0 0,0 0 0,0 0 0,-1 0 0,1 1-1,0-1 1,0 1 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 1 0,0-1 0,0 1 0,0-1-1,0 1 1,-1 0 0,1-1 0,0 1 0,0 0 0,0 1 7,5 2-35,-1 2-1,0-1 1,0 1 0,0 0 0,-1 0 0,0 0 0,0 1 0,0 0 0,-1 0-1,0 0 1,0 0 0,-1 1 0,0-1 0,0 1 0,-1 0 0,0 0-1,0 0 1,-1 0 0,0 0 0,0 0 0,-1 1 0,0-1 0,-1 0 0,1 0-1,-2 0 1,1 0 0,-1 0 0,0 0 0,-2 4 35,0-4 48,1 1 1,-2-1-1,1 0 1,-1 0-1,0-1 1,0 1-1,-1-1 1,0 0-1,-1-1 1,1 1-1,-1-1 1,0-1-1,-1 1 0,0-1 1,1 0-1,-1-1 1,-1 0-1,1 0 1,-1-1-1,1 0 1,-1-1-1,0 1 1,-7-1-49,13-2 5,-1 0 0,1-1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,0-1 0,-1 1 0,1-1 0,0 0 0,0 0 0,1 0 0,-1 0 0,0-1 0,1 1 0,-1-1 0,1 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0-1 0,1 1 0,-1 0 0,1 0 0,0-1 0,0 1 0,0-1 0,1 1 0,-1-1 0,1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,1-1 0,0 1 0,0-1 0,0 1 0,0 0 0,1-1 0,0 1 0,-1 0 0,1 0 0,1-1-5,1 1-4,-1 1 0,1-1 0,0 1 0,0 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0 1 0,0-1 0,1 0 0,-1 1 0,0 0 0,1 0 0,-1 0 0,0 1 0,1-1 0,-1 1 0,0 0 1,0 0-1,0 1 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,-1 1 0,1-1 0,-1 1 0,1 1 4,-3-3 8,0 0 1,0 1-1,0-1 1,0 0-1,-1 1 0,1-1 1,0 1-1,-1 0 1,1-1-1,-1 1 0,0-1 1,0 1-1,1 0 1,-1-1-1,0 1 0,0 0 1,-1-1-1,1 1 1,0-1-1,0 1 0,-1 0 1,1-1-1,-1 1 1,0-1-1,1 1 0,-1-1 1,0 1-1,0-1 1,0 0-1,0 1 0,0-1 1,0 0-1,0 0 1,-1 1-9,-47 36 151,46-36-147,-1 0-1,1 0 0,-1-1 1,1 1-1,-1-1 1,0 0-1,0 0 0,1 0 1,-1 0-1,0-1 1,0 1-1,0-1 0,0 0 1,0-1-1,0 1 1,0 0-1,1-1 0,-1 0 1,0 0-1,0 0 1,1-1-1,-1 1 0,1-1 1,-1 0-1,1 0 1,-1 0-1,1 0 0,0 0 1,0-1-1,0 0 1,1 1-1,-1-1 0,-1-2-3,2 2-186,-1 0-1,1 0 0,-1 0 1,1 0-1,0-1 0,0 1 1,1-1-1,-1 1 0,1-1 1,-1 0-1,1 0 0,0 1 1,1-1-1,-1 0 0,1 0 1,0 0-1,-1 0 0,2 0 1,-1 0-1,0 0 0,1-1 187,9-19-544</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink23.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-06-24T04:06:41.019"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#F6630D"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">-763 221 4864,'45'-31'6512,"-35"27"-5383,-12 8 494,0-3-1551,-1 0 0,0 0 1,1 1-1,-1-1 0,1 0 1,-1-1-1,0 0 0,0 1 1,1-1-1,-1 0 0,1 0 1,-1-1-1,0 1 0,0 0 1,1-1-1,-1 0 0,1-1 1,-1 1-1,1 0 0,-1 0 1,1 0-1,-1-1 0,1 1 1,0-1-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,1-1 1,0 1-1,0 0 0,-1-1 1,1 0-1,0 1 0,0-1 1,0 0-73,1 0 2,0 2 0,1-1 0,-1 1 0,0 0 0,1-1 0,-1 1 0,1 0 0,-1 0 1,1-1-1,0 1 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 1,0-1-1,1 0 0,-1 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,0 0 0,0 0 0,0-1 0,1 1 0,-1 0 1,0 0-3,44 6-119,-1 27 148,-43-32-24,0 0 0,-1 0 1,1 0-1,0 0 1,0 0-1,-1 0 1,0 0-1,1 1 0,-1-1 1,1 0-1,-1 1 1,0-1-1,1 0 1,-1 1-1,0-1 0,0 0 1,0 1-1,0-1 1,0 1-1,0-1 0,0 0 1,0 1-1,-1-1 1,1 0-1,0 1 1,-1-1-1,1 0 0,-1 0 1,1 2-1,0-2 1,-1 0-1,0 0 1,0 0-1,1 0 0,-1 0 1,-1 1-6,-5 5 44,1-1 0,-1 0 1,0 0-1,-1-1 0,0 0 0,1 1 1,-1-2-1,0 0 0,-1-1 0,-4 2-44,12-5 11,-1 1 0,1-1 0,0 1 0,-1-1 0,1 0-1,-1 0 1,0 0 0,0 0 0,1 0 0,-1 0-1,0-1 1,1 1 0,-1 0 0,1-1 0,0 0 0,-1 1-1,1-1 1,-1 0 0,1 1 0,-1-1 0,1 0-1,0 0 1,-1 0 0,1-1 0,0 1 0,1 0 0,-1 0-1,0-1 1,0 1 0,0-1 0,0 1 0,0 0-1,0-2 1,1 1 0,-1 0-11,0-7 48,0 0-1,0 0 1,1 0-1,0-1 0,1 1 1,0 0-1,1 0 1,0 0-1,0 0 1,2-8-48,-3 15-14,-1 0-1,1-1 1,0 1 0,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,1 0 0,-1 1 0,1-1 0,-1-1-1,0 2 1,0-1 0,1 1 0,0-1 0,0 1 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,-1 0-1,1 0 1,1 1 0,-1-1 0,0 1 0,0 0 0,1-1-1,-2 1 1,1 0 0,1 1 0,-1-1 0,0 0-1,0 0 1,1 1 0,-1 0 0,-1-1 0,1 1 0,0 0-1,1 0 15,0 1-23,-1-1 0,1 1 0,-1 0 0,0 0 0,1 0 0,-1 1 0,0 0 0,0-1 0,0 1 0,0-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 1 0,0 0 0,1-1 0,-1 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 2 23,-2 1 56,0-1 0,-1 0 1,0-1-1,1 0 0,-1 0 0,-1 0 0,1 0 0,0-1 0,-1 0 0,1 0 1,-6 2-57,9-4 15,0-1 1,0 1-1,0 0 1,-1-1-1,1 1 1,-1-1-1,1 0 1,-1 0-1,2 1 1,-2-2-1,1 1 1,-1 0-1,1-1 1,-1 1-1,1-1 1,0 1-1,0-1 1,0 0 0,-1 0-1,1-2 1,0 2-1,0 0 1,0-1-1,1 1 1,-1-1-1,0 1 1,0-1-1,1 0 1,-1 0-1,0 0 1,0-1-16,0-1 9,1-1 1,0 1-1,-1 0 1,1-1-1,0-1 1,0 2-1,0-1 1,1 0-1,0 1 0,0-1 1,0 0-1,0 1 1,1-1-1,-1 0 1,2-3-10,-2 5-15,1 1-1,-1 0 1,1-1 0,-1 1 0,1 0-1,0 0 1,0-1 0,-1 1 0,1 0 0,1 0-1,-1 0 1,0 0 0,1 0 0,0 1-1,-1-1 1,1 0 0,0 1 0,0-1 0,-1 0-1,1 1 1,0-1 0,0 1 0,0 0-1,0 0 1,0 0 0,1 1 0,-2-1 0,1 0-1,1 1 1,1-1 15,1 2 21,-2-1 0,1 1 0,0-1 0,0 1 0,0 0 0,-1 1 0,1-1 0,0 1 0,0-1 0,-2 2 0,2-1 0,0 1-1,-1-1 1,0 1 0,0-1 0,0 1 0,0 0 0,-1 0 0,1 1 0,0-1 0,-2 0 0,1 1 0,0-1 0,0 1 0,0 1 0,0-1 0,-1 0 0,1 1-21,-2-2 11,-1 1 1,1-1-1,-1 1 0,1 0 1,-1-1-1,0 1 1,0-1-1,-1 2 0,1-2 1,-1 0-1,1 0 1,-1 1-1,1-1 1,-2 0-1,1-1 0,0 1 1,-1 0-1,1-1 1,-1 1-1,1-1 0,-1 0 1,0 0-1,0 0 1,0 0-1,0 1 0,0-2 1,0 0-1,-1 1 1,1-1-1,0 0 0,0-1 1,-1 1-1,0-1 1,1 1-1,0-1 1,-1 0-1,1-1 0,-1 1 1,1-1-1,0 1 1,-1-1-1,1 0 0,-3-1-11,3 0 17,1-2-1,-2 2 1,1-1-1,0 1 1,0-1-1,2 0 1,-2 0-1,1 0 1,-1-1-1,1 1 1,0 0-1,0-1 1,0 0-1,1 1 1,0-2-1,0 1 0,0 0 1,0 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,1 0-1,-1 0 1,0 0-1,1-1 1,0 1-1,0 1 1,0-1-1,0 0 1,0 0-1,1 1 1,0-1-1,0 0 0,0 1 1,0 0-1,0 0 1,1-2-1,-1 2 1,0 1-1,1-1 1,0 0-1,1 1 1,-1-1-17,1 0-23,1 0 1,1 1-1,-2-1 1,1 1-1,1 0 1,-2 1-1,2-1 1,-1 1-1,0 0 1,1 1-1,-1-1 1,0 1-1,1 0 0,0 1 1,-1-1-1,0 1 1,1 0-1,-1 1 1,0-1-1,0 1 1,1 0-1,-2 1 1,1-1-1,0 1 1,-1 0-1,1 0 1,4 4 22,-8-5-2,0 0-1,0 0 1,0 1 0,0-1 0,0 0 0,0 0-1,0 1 1,-1-1 0,1 0 0,-1 1-1,1-1 1,-1 0 0,0 1 0,0-1 0,0 1-1,0-1 1,0 0 0,-1 1 0,1-1 0,-1 0-1,0 1 1,1-1 0,-1 1 0,0 0 0,0-1-1,0 0 1,0 0 0,0 0 0,0 0 0,-2 1 2,-49 56-20,51-58 20,-42 31-148,42-31 139,-1 0 0,1-1 0,0 1 0,0-1 0,-1 1-1,1-1 1,0 0 0,-1 0 0,1 1 0,-1-1 0,2 0 0,-1 0-1,-1 0 1,1 0 0,0-1 0,-1 1 0,1 0 0,0-1-1,-1 1 1,1-1 0,0 1 0,-1-1 0,1 1 0,1-1-1,-1 0 1,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0-1 0,1 1 0,-1 0 0,0 0-1,0-1 10,0-4 1,-1 1 0,1 0 0,0 0 0,0 0 0,1-1 0,-1 1 0,1 0 0,0 0 0,0-2 0,0 2 0,1 0 0,0-1 0,0 1 0,-1 0 0,2 0 0,0 0 0,0-1 0,0 1 0,0 0 0,1 1 0,0-1 0,-1 1 0,1 0 0,0 0 0,1 0 0,-1 0 0,1 0-1,2-3 36,0 1-1,-1 0 1,2 0 0,0 1-1,-1 1 1,1-1 0,-1 1-1,2 0 1,-1-1 0,1 2-1,0 0 1,-1 1 0,2 0-1,-2 0 1,1 1 0,5-1-36,-11 2-5,0-1 1,-1 1-1,1 0 1,0-1 0,0 1-1,0 0 1,0 0-1,0 0 1,0 1-1,0-1 1,-1 0-1,1 1 1,0-1 0,0 1-1,0 0 1,0 0-1,-1 0 1,1-1-1,0 2 1,-1-1-1,0 0 1,1 0 0,-1 1-1,1-1 1,-1 0-1,1 1 1,-1 0-1,0-1 1,0 2-1,0-1 1,0-1 0,0 1-1,0 0 1,0 0-1,-1 0 1,0 0-1,0 0 1,1 0-1,-1 0 1,0 0 0,1 0-1,-1 2 5,-2 3 16,0 0 0,-1 1 0,-1-2 0,1 1 0,-1 0 0,1-1 0,-1 0 0,-1 0 0,0 0 0,1 0 0,-1-1 0,-1 0 0,1 0 0,-1-1 0,-3 3-16,4-3 8,0 1 59,0 1 0,-1-1-1,-1 0 1,2-1 0,-2 0 0,0 0 0,1 0 0,-1-1-1,1 0 1,-2-1 0,1 0 0,0 0 0,0 0 0,0-1 0,-1 1-1,-3-2-66,8 0 25,0-2 0,1 1 0,0-1 0,-1 1 0,1 0 0,-1-1-1,1 1 1,0-1 0,-1 0 0,2 0 0,-1 0 0,0 0 0,0 0-1,0 0 1,1 0 0,-1-1 0,1 1 0,-1-1 0,1 1 0,0-1 0,1 0-1,-1 1 1,0-2 0,0 1 0,1 0 0,-1 0 0,1 0 0,0 1-1,0-3-24,-1-1 30,1-1 0,0 1-1,1-2 1,-1 2 0,1 0 0,1-1-1,-1 1 1,0 0 0,1 0-1,0 0 1,1-1 0,2-3-30,-4 8-3,0 0 1,0 1-1,-1-1 1,2 0-1,-1 0 1,1 1-1,-1-1 1,1 1-1,0-1 1,-1 1-1,1 0 1,0-1-1,0 1 0,-1 0 1,1 0-1,0 0 1,0 1-1,0-1 1,1 0-1,-1 1 1,0 0-1,-1-1 1,1 1-1,1 0 1,-1 0-1,0 0 1,0 0-1,1 1 1,-1-1-1,-1 0 1,1 1-1,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0 0-1,-1 1 1,1-1-1,0 0 1,-1 1-1,1-1 1,0 1-1,-1 0 0,1-1 1,-1 1-1,0 0 1,0 0-1,0 0 1,0 0-1,-1 0 1,1 0-1,0 1 3,0 2 18,-1 0 0,0 0-1,0 0 1,0 0-1,0-1 1,-1 1 0,0 0-1,0-1 1,1 1-1,-2-1 1,0 2 0,1-2-1,-1 0 1,-1 0-1,1 0 1,-1 0 0,1 0-1,0 0 1,-2-1-1,-1 3-17,5-6 13,0 1 0,0-1 0,0 1 0,-1 0 0,1-1 1,0 2-1,-1-2 0,1 1 0,0-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,0 0 0,0 1 0,-1-1 0,1 0 0,-1 1 0,0-1 0,1 0 0,-1 0 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1-1 0,-1 1 0,1 0 0,-1 0 0,0-1 1,1 1-1,-1 0 0,1-1 0,-1 1 0,1 0 0,0-1 0,0 1 0,-1-1 0,1 1 0,-1-1 0,1 1 0,-1-1-13,-8-37 213,9 34-213,0 0-3,-1-1-1,1 2 1,-1-1-1,1 0 1,0 0-1,1 0 1,-1 0 0,0 1-1,1-1 1,0 0-1,0 0 1,0 1 0,1-2-1,-1 2 1,1-1-1,0 1 1,0-1 0,-1 1-1,1 0 1,1 0-1,-1 0 1,1 0-1,0 1 1,-1-1 0,2 0 3,0 3 2,1 0 0,-1 1 0,1-1 0,-1 1 0,1 1 0,-1-1 0,0 0 0,1 1 0,-1 0 0,-1 0 0,2 1 0,-1-1 0,0 1 0,-1 0 0,0 0 0,1 0 0,-1 0 0,1 1 0,-2-1 0,1 2 0,1 0-2,-2-3 2,0 1 0,0-1 0,0 0 0,0 0 0,-1 1 0,0-1 0,1 1 1,-1 0-1,0-1 0,1 1 0,-1 0 0,0 0 0,-1 0 0,1 1 0,0-2 0,-1 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,-1 1-2,-3 3 24,-1 1-1,-1-1 1,1-1 0,-1 1-1,0-1 1,0 1 0,-1-2-1,0 0 1,0 0 0,0-1-1,-1 0 1,1 0 0,-1-1-1,1-1 1,-2 1 0,-5 0-24,13-3 4,-2 0 0,0 0 0,1 0 0,-1 0 1,1 0-1,0-1 0,-1 0 0,1 1 0,-1-1 0,2-1 1,-2 1-1,1 0 0,0-1 0,-1 0 0,2 0 1,-1 0-1,0 0 0,0 0 0,1-1 0,-1 1 0,1-1 1,0 0-1,0 1 0,0-1 0,0 0 0,0-2 0,0 2 1,0 0-1,1 0 0,0-1 0,0 1 0,0-1 1,0 1-1,1-1 0,-1 0 0,1 1 0,0-1-4,-2-5-13,1 2 0,1-1 0,-1 1 0,1-1-1,1 1 1,-1-2 0,1 2 0,1 0 0,-1-1-1,1 1 1,-1 0 0,2-1 0,0 1 0,0 0-1,0 0 1,1 1 0,-1-1 0,2 1 0,2-5 13,-5 9-6,0 1 1,0-1-1,1 0 1,-1 1-1,1-1 1,-1 1 0,1 0-1,-1 0 1,0 0-1,1 0 1,0 1-1,0-1 1,0 1-1,-1-1 1,0 1 0,1 0-1,0 0 1,0 0-1,0 1 1,-1-1-1,1 1 1,-1-1-1,1 1 1,0 0 0,0 0-1,-2 0 1,2 1-1,-1-1 1,1 1-1,1 1 6,1 0-47,0 1 1,0 1-1,0 0 0,-1-1 0,0 1 0,1 0 0,-1 0 1,-1 1-1,0-1 0,1 1 0,-1 1 0,1 4 47,-2-6 18,-1-1-1,0 0 0,0 1 1,0-1-1,0 1 0,-1 0 1,1 0-1,-1 0 0,-1-1 1,1 1-1,-1-1 0,1 1 1,-1-1-1,0 1 0,-1-1 1,1 1-1,0-1 0,-1 1 1,0-1-1,0 0 0,-1-1 1,1 1-1,-1 0 0,-2 2-17,5-5 7,-1-1 0,1 1 0,-1-1-1,1 1 1,-1-1 0,1 0 0,-1 1-1,0-1 1,1 0 0,-1 0-1,1 1 1,-1-1 0,0 0 0,1 0-1,-1 0 1,0 0 0,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0 0,0 0-1,1 0 1,0-1 0,-1 1 0,1 0-1,-1 0 1,1-1 0,-1 1 0,1 0-1,-1-1 1,0 1 0,1 0 0,-1-1-1,1 1 1,-1-1 0,1 1 0,0-1-1,-1 1 1,1-1 0,-1 1-1,1-1 1,0 1 0,0-1 0,-1 0-1,1 1 1,0-1 0,0 0 0,0 1-1,-1-1-6,-7-38 134,7 37-119,4-83-90,-2 83 72,-1 0 0,0-1 0,1 1-1,0 0 1,-1 0 0,1 0 0,1 0 0,-1 0 0,0 0 0,0 0-1,1 0 1,-1 0 0,1 1 0,0-1 0,-1 1 0,0-1 0,1 1 0,0 0-1,0-1 1,0 1 0,0 0 0,0-1 0,0 1 0,0 1 0,-1-1-1,2 0 1,-1 1 0,0 0 0,1-1 0,-1 1 0,0 0 0,-1 0-1,2 0 1,0 1 3,0-1 4,0 1 0,1-1-1,-2 1 1,1 0 0,0 1-1,0 0 1,0-1 0,0 1-1,-1-1 1,1 1 0,0 0-1,0 0 1,-1 0 0,1 0-1,-2 1 1,1-1 0,0 1 0,0 0-1,0-1 1,0 1 0,0 0-1,-1 0 1,1 0 0,-1 0-1,-1 1 1,1 0 0,0-1-1,0 0 1,0 4-4,-3 0 16,0 0 0,-1 0 1,0 1-1,-1-1 0,1 0 0,0 0 1,-2-1-1,1 0 0,-1 0 0,0 1 1,0-2-1,-1 1 0,2-1 0,-3-1 1,1 1-1,1-1 0,-2 0 0,0 0 1,1-1-1,-1 1 0,1-1 0,-3 0-16,8-2-237,-1-1 1,0 1-1,1 0 0,-1 0 0,0-1 0,0 1 0,0-1 0,0 1 1,0-1-1,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0-1 0,0 1 1,0-1-1,0 1 0,0-1 0,1 1 0,-1-1 0,0 0 0,0 0 1,1 0-1,-1 0 0,0-1 0,1 1 0,-1 0 0,0-2 237,-5-18-858</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink24.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-06-24T04:06:41.020"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#B99C4B"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">62 83 6400,'23'-40'6647,"10"9"-5140,-33 30-1493,1 1 0,0 0 0,-1 0 0,1 0 0,-1-1 0,1 1 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 1 0,1-1 0,-1 0-1,1 0 1,0 0 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 0,0 0 0,1-1 0,-1 1 0,0-1 0,0 1-1,0 0 1,0-1 0,1 1 0,-1-1 0,0 1 0,0 0 0,0-1 0,0 1 0,-1 0-14,3 37 237,-3-28-1,0 1 1,-1 0-1,1-1 1,-2 1-1,0-1 0,0 0 1,-1 0-1,0 0 1,-1 0-1,0-1 1,0 0-1,-2 3-236,6-11 42,0 0-1,0-1 1,0 1-1,0 0 1,0 0-1,0 0 1,0-1 0,0 1-1,0 0 1,0-1-1,0 1 1,0-1-1,0 1 1,-1-1-1,1 0 1,0 1 0,0-1-1,0 0 1,-1 0-1,1 0 1,0 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,0-1-1,0 1 1,-1 0-1,1-1 1,0 1-1,0-1 1,0 0 0,0 1-1,0-1 1,0 0-1,0 1 1,0-1-1,0 0 1,0 0-1,0 0 1,0 0 0,1 0-1,-1 0 1,0 0-1,1 0 1,-1 0-1,1 0 1,-1 0 0,1 0-1,-1-1 1,1 1-1,0 0 1,-1 0-42,0-5-2,-1 1 0,1-1 0,-1 0 0,1 1-1,1-1 1,-1 0 0,1 1 0,0-1 0,1 0 0,-1 0 0,1 1 0,0-1 0,1-1 2,-1 6-3,0 0 1,1 1-1,-1-1 1,0 1-1,0-1 1,1 1-1,-1 0 0,0-1 1,1 1-1,-1 0 1,0 0-1,1 0 1,-1 0-1,0 0 0,1 0 1,-1 0-1,0 0 1,1 1-1,-1-1 1,0 1-1,0-1 0,1 1 1,-1-1-1,0 1 1,0-1-1,0 1 0,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,0 0 2,0 0-11,68 66-384,-67-64 405,-1 0 1,0 0-1,-1 1 0,1-1 1,0 1-1,-1-1 0,0 1 1,0-1-1,0 0 0,0 1 1,0-1-1,-1 1 0,0-1 1,1 1-1,-1-1 0,-1 0 0,1 0 1,0 1-1,-1-1 0,1 0 1,-1 0-1,0 0 0,0-1 1,0 1-1,-1 0 0,1-1 1,-1 1-1,1-1 0,-1 0 1,0 0-1,0 0 0,0 0 1,0-1-1,0 1 0,0-1 1,0 1-1,0-1 0,-1 0 0,1-1 1,-1 1-1,1 0 0,0-1 1,-1 0-1,1 0 0,-1 0 1,-3 0-11,3-3 14,-1 1 1,1 0 0,0-1 0,0 0-1,0 0 1,0 0 0,0 0-1,0-1 1,1 0 0,0 1 0,0-1-1,0-1 1,0 1 0,0 0 0,1-1-1,0 1 1,0-1 0,0 1-1,1-1 1,-1 0 0,1 0 0,0 0-1,1 0 1,-1 0 0,1-3-15,0 2 2,-1 0 1,2 0-1,-1-1 0,1 1 1,0 0-1,0 0 1,0 0-1,1 0 1,0 0-1,0 1 1,1-1-1,0-1-2,-2 5 0,1 0 1,-1-1-1,0 1 1,1 0-1,0 0 1,-1 0-1,1 1 1,0-1-1,0 0 0,0 1 1,0-1-1,0 1 1,0 0-1,0-1 1,1 1-1,-1 0 1,1 0-1,-1 1 0,0-1 1,1 0-1,-1 1 1,1 0-1,-1-1 1,1 1-1,-1 0 1,1 0-1,0 1 0,-1-1 1,1 0-1,1 1 0,-1 1-3,0-1 0,0 0-1,0 1 1,-1-1 0,1 1 0,0 0-1,-1 0 1,1 0 0,-1 0-1,0 0 1,0 1 0,0-1 0,0 1-1,0 0 1,0-1 0,-1 1-1,1 0 1,-1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,-1 0 1,1 0 0,-1 1 0,0-1-1,0 0 1,0 0 0,-1 0-1,1 1 1,-1-1 0,1 0-1,-1 0 1,0 0 0,0 0 0,-1 0-1,1 0 1,-1 0 0,1-1-1,-1 1 1,0 0 0,0-1 0,0 0-1,0 1 1,0-1 0,-3 2 3,4-2 44,-1 0 0,1 0 0,-1 0-1,1-1 1,-1 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,-1 0 0,1 0 0,0-1 0,-1 1 0,1 0 0,0-1-1,-1 1 1,1-1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1-1 0,1 1 0,-1-1 0,1 1 0,0-1 0,-1 0 0,1 0 0,0 0 0,0 0-1,0-1 1,0 1 0,0 0 0,0-1 0,0 0 0,0 1 0,1-1 0,-1 0-44,0-4 12,0 0 0,1 0 0,-1 0 0,1 0 0,1 0 0,-1 0-1,1 0 1,0-1 0,1 1 0,-1 0 0,1 0 0,0 0 0,1 0 0,0 0 0,0 0 0,0 0 0,3-4-12,-3 6-20,0 1 1,0 0-1,1 0 1,-1 0 0,1 0-1,0 1 1,0-1 0,0 1-1,0-1 1,0 1-1,0 0 1,1 0 0,-1 1-1,1-1 1,-1 1-1,1 0 1,0 0 0,-1 0-1,1 0 1,0 0 0,0 1-1,0 0 1,0 0-1,0 0 1,-1 0 0,1 0-1,0 1 1,0 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,-1 1 0,1 0-1,-1 0 1,0 0-1,1 0 1,-1 0 0,0 1-1,0-1 1,-1 1 0,1 0-1,0-1 1,-1 2-1,0-1 1,1 0 0,-1 0-1,-1 1 1,1-1-1,0 1 1,-1-1 0,1 4 19,-1 4 10,0-1 1,-1 1 0,-1-1-1,0 1 1,0-1 0,-1 1-1,0-1 1,-1 0 0,0 0-1,0 0 1,-1 0 0,-1-1-1,0 1 1,0-1 0,-1 0-1,-3 4-10,9-11 17,-1-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,0 1 0,0-1-1,0 1 1,0-1 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 1 0,1-2 0,0 1-1,-1 0 1,1 0 0,-1 0 0,0-1 0,1 1 0,-1-1 0,1 1 0,-1-1 0,0 0-1,1 1 1,-1-1 0,0 0 0,1 0 0,-1 0 0,0 0 0,0-1 0,1 1 0,-1 0-1,0-1 1,1 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 0-17,-2-4 9,0-1 1,0 1 0,0-1-1,1 0 1,0 1 0,1-1-1,-1 0 1,1 0 0,0 0-1,0 0 1,1 0 0,0-1-1,0 1 1,0 0 0,1 0-1,1-2-9,-2 1-5,0 1 0,1 0 0,0 1 0,0-1-1,1 0 1,0 0 0,0 0 0,0 1 0,1-1-1,-1 1 1,1 0 0,1-1 0,-1 1 0,1 1-1,0-1 1,0 1 0,0-1 0,0 1 0,1 0 0,0 1-1,0-1 1,0 1 0,0 0 0,0 0 0,1 0-1,-1 1 1,1 0 0,0 0 0,0 0 0,0 1-1,-1 0 1,1 0 0,0 1 0,1-1 0,-1 1-1,0 1 1,2-1 5,-5 1-13,1-1 0,0 1 0,-1 0 0,1 0 0,-1 0 0,1 1 0,-1-1 0,0 1-1,1-1 1,-1 1 0,0 0 0,0 1 0,0-1 0,0 0 0,-1 1 0,1 0 0,-1-1 0,1 1 0,-1 0-1,0 0 1,0 1 0,0-1 13,-2 4 7,0 0 0,0 0 0,-1 0 0,1 0 0,-2 0 0,1-1 0,-1 1-1,0 0 1,0-1 0,-1 1 0,0-1 0,0 0 0,0 0 0,-1 0 0,0 0 0,0 0-1,0-1 1,-1 0 0,0 0 0,0 0 0,0-1 0,-1 1 0,1-1 0,-2 0-7,5-2 15,-1 0 0,1 0 1,-1-1-1,1 1 1,-1-1-1,0 1 0,0-1 1,0 0-1,1 0 0,-1 0 1,0 0-1,-1-1 1,1 1-1,0-1 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0-1 1,0 0-1,0 1 0,0-1 1,0 0-1,0 0 0,0-1 1,0 1-1,1-1 1,-1 1-1,1-1 0,-1 0 1,1 0-1,-1 0 1,1 0-1,0 0 0,0-1 1,0 1-1,0-1 0,0 1 1,1-1-1,-1 1 1,1-1-1,0-1-15,-2-2 2,0-1 0,0 0 0,1 0-1,0 0 1,1 0 0,0 0 0,0 0 0,0 0 0,1 0 0,0 0-1,0-1 1,1 1 0,0 0 0,0 0 0,1 0 0,0 0 0,0 0 0,0 1-1,1-1 1,2-3-2,-2 8-12,0-1 0,0 1 0,1-1 0,-1 1 0,1 0 0,-1 1 0,1-1-1,0 1 1,0-1 0,0 1 0,-1 0 0,1 0 0,0 1 0,0-1 0,0 1 0,0 0-1,1 0 1,-1 0 0,0 1 0,0-1 0,-1 1 0,1 0 0,0 0 0,0 1 0,0-1 0,0 1-1,-1 0 1,1 0 0,-1 0 0,0 0 0,1 0 0,-1 1 0,0-1 0,0 1 0,0 0-1,-1 0 1,1 1 12,0 1-4,-1-1-1,0 2 1,0-1-1,0 0 1,0 0-1,-1 1 1,0-1-1,0 1 0,0-1 1,-1 1-1,0-1 1,0 1-1,0-1 1,-1 1-1,1-1 1,-1 1-1,-1-1 1,1 1-1,-1-1 0,0 0 1,0 0-1,-1 0 1,1 0-1,-1 0 1,0 0-1,-1-1 1,-2 4 4,-33 29 278,38-36-267,0 0-1,-1-1 0,1 1 1,0 0-1,0 0 0,0-1 1,-1 1-1,1-1 0,0 1 1,0-1-1,-1 0 1,1 1-1,0-1 0,-1 0 1,1 0-1,-1 0 0,1 0 1,0 0-1,-1 0 0,1 0 1,0-1-1,-1 1 0,1 0 1,0-1-1,-1 1 0,1-1 1,0 1-1,0-1 0,0 0 1,-1 1-1,1-1 0,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,1 0-11,-4-7 1,0 0 0,1 0 0,1 0 1,-1 0-1,1-1 0,1 1 1,0 0-1,0-1 0,0 0 0,1 1 1,0-1-1,1 1 0,0-1 0,0 1 1,1-1-1,0 1 0,1 0 0,-1 0 1,1 0-1,1 0 0,3-5-1,-6 9-5,1 0 0,-1 1 1,1-1-1,0 1 0,0 0 0,1-1 0,-1 1 0,1 0 0,-1 0 0,1 0 0,0 1 0,0-1 1,0 1-1,0 0 0,1-1 0,-1 1 0,0 1 0,1-1 0,0 0 0,-1 1 0,1 0 0,0 0 1,0 0-1,0 0 0,0 1 0,-1-1 0,1 1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 1 1,0 0-1,0 0 0,-1 0 0,1 0 0,2 2 5,-4-2-7,1 0 1,0 1-1,-1 0 0,1-1 1,-1 1-1,1 0 1,-1 0-1,0 1 0,0-1 1,0 0-1,0 1 1,0-1-1,0 1 0,-1-1 1,1 1-1,-1 0 0,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,-1 0 1,1 0-1,-1 0 0,0 0 1,0 0-1,0 0 1,0 0-1,-1 2 7,-2 5 25,0 1-1,-1-1 1,0 0 0,-1 0-1,0 0 1,-1-1 0,0 0-1,0 0 1,-1 0 0,0-1-1,-1 0 1,0 0 0,0-1-1,0 0 1,-1 0 0,-5 2-25,12-8 4,0 1 1,0-1 0,0 0-1,0 0 1,-1-1 0,1 1-1,0 0 1,-1-1 0,1 1 0,0-1-1,-1 0 1,1 0 0,0 0-1,-1 0 1,1 0 0,0 0-1,-1-1 1,1 1 0,0-1-1,0 1 1,-1-1 0,1 0 0,0 0-1,0 0 1,0 0 0,0-1-1,0 1 1,0 0 0,0-1-1,0 1 1,1-1 0,-1 0-1,1 0 1,-1 1 0,1-1 0,0 0-1,-1 0 1,1 0 0,0-1-1,0 1 1,0 0 0,1 0-1,-1 0 1,1-1 0,-1 1 0,1 0-1,0-1 1,-1 1 0,1 0-1,1-2-4,-2-5 3,0 1-1,1 0 0,0-1 0,0 1 1,1-1-1,0 1 0,1 0 1,0 0-1,0 0 0,1 0 0,0 0 1,0 0-1,1 1 0,0-1 1,0 1-1,1 0 0,0 0 0,0 1 1,0-1-1,1 1 0,0 0-2,-3 5-9,0 0 0,1 0 0,-1 0-1,0 1 1,0-1 0,0 1 0,0 0-1,1 0 1,-1 0 0,0 0 0,0 0-1,0 1 1,0 0 0,1-1 0,-1 1-1,0 0 1,0 1 0,0-1 0,-1 0-1,1 1 1,0 0 0,0-1 0,-1 1-1,1 0 1,-1 1 0,0-1 0,0 0-1,1 1 1,-2-1 0,1 1 0,0-1-1,0 1 1,-1 0 0,1 0 0,-1 0 0,0 0-1,0 0 1,0 0 0,0 0 0,-1 0-1,1 0 1,-1 1 0,0-1 0,0 0-1,0 3 10,0 1 23,0 1 1,0-1-1,0 0 0,-1 1 0,0-1 0,-1 0 0,1 0 0,-1 0 0,-1 0 0,1 0 1,-1 0-1,-1-1 0,1 0 0,-1 1 0,0-1 0,0 0 0,-1-1 0,0 1 0,0-1 1,0 0-1,0 0 0,-1 0 0,0-1 0,-3 2-23,7-5 12,1-1 0,-1 0-1,1 0 1,-1 0 0,1 1 0,-1-1 0,1 0-1,-1-1 1,1 1 0,-1 0 0,1 0 0,-1-1-1,1 1 1,-1-1 0,1 1 0,-1-1 0,1 0 0,0 1-1,-1-1 1,1 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0-1-1,0 1 1,0 0 0,1-1 0,-2 0-12,-17-51 70,16 44-70,1-1 0,0 1 1,0 0-1,1-1 0,1 1 0,-1-1 1,1 1-1,1-1 0,0 1 0,0-1 1,1 1-1,0 0 0,0 0 0,1 0 1,1 0-1,-1 0 0,1 0 0,1 1 1,0 0-1,0 0 0,2-2 0,-4 8-17,1 0-1,-1 0 0,1 1 0,0 0 1,-1-1-1,1 1 0,0 1 0,0-1 1,0 0-1,0 1 0,0 0 0,-1 0 1,1 0-1,0 0 0,0 1 0,0 0 1,0-1-1,0 2 0,-1-1 1,1 0-1,0 1 0,-1-1 0,1 1 1,-1 0-1,0 0 0,1 0 0,-1 1 1,0-1-1,0 1 0,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 1,0 0-1,0 1 0,0-1 0,0 1 1,-1-1-1,0 1 0,1 0 0,-1-1 1,0 4 17,-3 0 8,0 0 1,-1 0 0,0-1-1,0 1 1,-1-1 0,1 0 0,-1 0-1,-1 0 1,1 0 0,-1-1-1,0 0 1,0 0 0,-1 0-1,1 0 1,-1-1 0,0 0 0,0 0-1,0-1 1,-3 1-9,7-2 19,0 0-1,0 0 1,-1 0 0,1-1-1,0 1 1,-1-1 0,1 1-1,-1-1 1,1 0 0,-1 0-1,0 0 1,0 0 0,1-1-1,-1 1 1,0-1 0,0 1-1,0-1 1,0 0 0,1 0-1,-1-1 1,0 1 0,0 0-1,0-1 1,1 0 0,-1 0-1,0 1 1,1-2 0,-1 1-1,0 0 1,1 0 0,0-1-1,-1 0 1,1 1 0,0-1-1,0 0 1,0 0 0,0 0-1,-2-2-18,3 0 1,-1-1-1,1 1 1,-1-1 0,1 1-1,1-1 1,-1 0 0,1 1-1,0-1 1,0 0-1,0 1 1,0-1 0,1 0-1,0 1 1,0-1 0,0 1-1,1-1 1,-1 1-1,1-1 0,-1 3-1,0 0 0,0 0 1,0 1-1,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,1 1 0,-1-1 0,1 1 0,-1-1 0,1 1 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 1,0 1-1,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,0 0 0,0 0 0,0-1 1,0 2 0,1-1-5,1 1 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 1 1,1-1-1,-1 1 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,-1 0 1,1 1-1,-1-1 0,1 0 0,-1 1 0,0-1 0,-1 1 0,1 0 0,0-1 1,-1 1-1,0 0 0,0-1 0,0 1 0,0-1 0,-1 1 0,1 0 0,-1-1 1,0 1-1,0-1 0,-1 1 0,0 1 5,0 1 34,-1 0 0,1 0 0,-2 0 0,1 0 0,0-1 0,-1 0 0,0 1-1,-1-1 1,1-1 0,-1 1 0,0-1 0,0 1 0,0-1 0,0-1 0,-1 1 0,0-1 0,1 0 0,-1 0 0,0-1 0,-1 1 0,1-2 0,0 1-34,3-2 1,0-1 0,1 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,0 0 0,-1 0 1,1-1-1,0 1 0,0-1 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 1,1 0-1,-1 0 0,1 0 0,0-1 0,0 1 1,-1-1-1,1 0-1,-10-40-3820,22-6-1284,3 14 4059</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink25.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-06-24T04:06:41.021"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#00A0D7"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">74 116 5504,'1'-1'107,"-1"1"0,1-1 0,-1 1 0,1-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,1 0 1,0 0-1,-1 0 0,1-1 0,-1 1 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 1 0,-1-1 0,1 0 0,-1 0 0,1 1 0,-1-1 1,1 0-1,0 0 0,-1 1 0,1-1 0,-1 1 0,0-1 0,1 0 0,-1 1 0,1-1 0,-1 1-107,48 49 309,-46-46-244,0 0-1,-1-1 0,1 1 0,-1 0 1,0 0-1,0 0 0,-1 1 1,1-1-1,-1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,-1 1 1,1-1-1,-1 0 0,0 0 0,-1 0 1,0 2-65,1-5 60,1 0 0,-1 0 0,1 0 0,0-1 0,-1 1 0,0 0 0,1 0 0,-1-1 0,1 1 0,-1-1 0,0 1 0,0 0 0,1-1 0,-1 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 1,0 1-1,1 0 0,-1 0 0,0-1 0,0 1 0,0-1 0,1 1 0,-1-1 0,0 0-60,-26-29 1452,24 22-1303,0 0 1,0-1-1,1 1 0,0-1 1,1 1-1,0-1 0,0 1 0,1-1 1,0 0-1,0 0 0,1 1 1,0-1-1,1 1 0,0-1 1,0 1-1,1-1 0,0 1 1,0 0-1,4-7-149,-4 13-8,-1 0 0,0 0 0,1 0 0,-1 0 0,1 1 0,0-1 0,-1 1 0,1-1 0,0 1-1,0 0 1,0 0 0,0 0 0,0 1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 1 0,0-1 0,1 0 0,-1 1 0,0 0 0,0-1 0,0 1-1,-1 0 1,1 1 0,0-1 0,0 0 0,0 1 0,-1 0 0,1-1 0,-1 1 0,1 0 0,-1 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1-1,0 2 9,0-1-39,-1 0-1,1 0 0,0 1 0,-1-1 0,0 0 0,0 1 0,0-1 0,0 1 1,-1-1-1,1 1 0,-1 0 0,0-1 0,0 1 0,0-1 0,-1 1 1,1 0-1,-1-1 0,0 1 0,0-1 0,0 1 0,-1 0 40,-1 4 76,0-1 0,-1 1 0,0-1 0,0 0 0,0 0 0,-1-1 0,0 1 0,-1-1 0,1 0 0,-1 0 0,-1-1 0,1 0 0,0 0 0,-1 0 0,0-1 0,0 0 0,-1 0 0,1-1 0,-1 0 0,0 0 0,0-1 0,0 0 0,0-1 0,-4 1-76,10-2 22,-1 0 0,1-1 0,0 0-1,-1 1 1,1-1 0,0 0 0,-1 0 0,1 0 0,0-1 0,0 1-1,0 0 1,0-1 0,0 1 0,0-1 0,1 0 0,-1 0-1,0 0 1,1 1 0,0-1 0,-1-1 0,1 1 0,0 0 0,0 0-1,0 0 1,0-1 0,0 1 0,1 0 0,-1-1 0,1 1-1,-1-1 1,1 1 0,0-1 0,0 1 0,0 0 0,0-1 0,1 1-1,-1-1 1,1 1 0,-1-1 0,1 1 0,0 0 0,0 0-1,0-1 1,0 1 0,0 0 0,1 0 0,-1 0 0,1 0-1,-1 0 1,1 0 0,0 1 0,1-2-22,1 2-11,0 0 0,0 1 0,0-1 0,0 1-1,0 0 1,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0 1-1,-1-1 1,1 1 0,0-1 0,2 3 11,1-1-41,24 9-133,-19-9 82,-1 2 1,0-1-1,0 1 1,-1 0-1,0 1 1,0 1-1,0 0 1,7 6 91,-16-12-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 1 1,0-1-1,0 1 1,0-1 0,0 1-1,0-1 1,0 1-1,0-1 1,-1 1-1,1 0 1,-1-1-1,1 1 1,-1 0-1,0 0 1,0-1-1,0 1 1,0 0-1,0 0 1,0-1 0,0 1-1,0 0 1,-1 0-1,1-1 1,-1 1-1,1 0 1,-1-1-1,0 1 1,1-1-1,-1 1 1,0 0-1,0-1 1,0 0-1,0 1 1,0-1-1,-1 0 1,1 1 0,0-1-1,-2 1 1,-1 1 33,-1 0-1,1 0 1,-1 0 0,0-1 0,0 0-1,0 1 1,0-2 0,0 1-1,0-1 1,0 1 0,-1-2-1,1 1 1,-4 0-33,4-1 64,0 0 1,1 0-1,-1 0 1,1-1-1,-1 0 1,1 1-1,0-2 0,-1 1 1,1 0-1,0-1 1,0 0-1,0 0 1,0 0-1,0-1 0,0 1 1,0-1-1,1 0 1,-1 0-1,1 0 0,0 0 1,0-1-1,0 1 1,1-1-1,-1 0 1,1 0-1,0 0 0,0 0 1,0 0-1,0 0 1,1 0-1,0-1 1,-1 1-1,2-1 0,-1 1 1,1-1-1,-1 1 1,1-1-1,0-1-64,3-2-8,-1 1 1,1 0-1,0 0 1,0 0-1,0 0 1,1 0-1,0 1 1,1 0-1,0 0 1,0 0-1,0 0 1,0 1-1,1 0 0,0 0 1,0 0-1,0 1 1,1 0-1,0 0 1,-1 0-1,1 1 1,0 0-1,1 1 1,-1-1-1,0 2 0,1-1 1,0 1-1,-1 0 1,1 0-1,6 1 8,-11 0-39,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 1 0,1-1-1,-1 1 1,0-1 0,1 1 0,-1 0-1,0 0 1,1 0 0,-1 0-1,0 1 1,0-1 0,0 0 0,0 1-1,0 0 1,0-1 0,-1 1-1,1 0 1,0 0 0,-1 0 0,0 0-1,1 0 1,-1 0 0,0 0-1,0 1 1,0-1 0,0 0 0,-1 1-1,1-1 1,-1 1 0,1-1-1,-1 1 1,0-1 0,0 1 0,0-1-1,0 0 1,0 1 0,-1-1 39,1 5 10,-1-1-1,0 0 1,-1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,-1 0 0,0-1-1,0 1 1,-1-1 0,0 0 0,1 0 0,-2 0-1,1-1 1,-1 1 0,1-1 0,-1 0-1,0 0 1,0-1 0,-1 1 0,1-1 0,-1 0-1,-1 0-9,5-3 6,1 0 0,-1 1-1,0-1 1,0 0-1,1 0 1,-1 0-1,0 0 1,0 0 0,1 0-1,-1 0 1,0-1-1,0 1 1,1-1-1,-1 1 1,1-1 0,-1 0-1,0 1 1,1-1-1,-1 0 1,1 0-1,0 0 1,-1 0 0,1-1-1,0 1 1,-1 0-1,1 0 1,0-1 0,0 1-1,0-1 1,0 1-1,1-1 1,-1 1-1,-1-2-5,-14-61 136,16 59-118,-1 0 0,1 0 1,0 1-1,0-1 0,1 0 0,-1 1 0,1-1 0,0 0 0,0 1 0,0-1 0,1 1 0,0-1 0,0 1 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,0 1 0,1-1 0,-1 1 1,1 0-1,-1 0 0,1 0 0,3-1-18,2 0-4,1 1 1,0 0-1,0 0 0,0 1 1,0 1-1,0 0 1,0 0-1,0 0 1,1 2-1,-1-1 1,0 1-1,0 1 0,0 0 1,0 0-1,6 3 4,-12-4-34,0 0 0,-1 1 0,1-1 0,-1 1 0,1 0 0,-1 0 0,0 0 0,0 1 0,0-1 0,0 1 0,0 0 0,-1-1 0,1 1 0,-1 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,-1 1 0,1-1 0,-1 1 0,0 0 0,0-1 0,-1 1 0,1 0 0,-1 0 0,0 0-1,0 0 1,0 0 0,0-1 0,-1 1 0,1 0 0,-1 0 0,0 0 0,0-1 0,0 1 0,-1-1 0,0 1 0,1-1 0,-1 1 0,-1 0 34,-3 5 58,-1 0 0,-1 0 0,1-1 0,-1 0 0,-1 0-1,1-1 1,-1 0 0,-1 0 0,1-1 0,-1 0 0,0-1 0,0 0 0,-1-1 0,-10 3-58,19-6 19,-1 0 0,0 0 0,1 0 0,-1 0 0,0-1 0,0 1 0,0-1 1,0 0-1,1 0 0,-1 0 0,0 0 0,0-1 0,0 1 0,0-1 0,1 1 0,-1-1 1,0 0-1,0 0 0,1 0 0,-1-1 0,1 1 0,-1-1 0,1 1 0,0-1 0,-1 0 1,1 0-1,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0-1 0,1 1 0,0-1 1,-1 1-1,0-4-19,-1-3 31,0-1 1,0 0 0,1-1 0,0 1 0,1 0-1,0 0 1,1-1 0,0 1 0,1-1 0,0 1-1,0 0 1,1 0 0,1 0 0,-1 0-1,2 0 1,-1 0 0,1 0 0,1 1 0,0 0-1,0 0 1,1 0 0,0 1 0,0 0 0,1 0-1,2-2-31,-6 7 2,-1 1-1,1 0 0,0-1 0,0 1 0,0 0 0,0 0 1,0 0-1,0 1 0,0-1 0,1 1 0,-1 0 1,0 0-1,1 0 0,-1 0 0,1 1 0,-1-1 0,1 1 1,0 0-2,2 1-25,0 1 1,0 0-1,0 1 1,0-1-1,-1 1 0,1 0 1,-1 1-1,1-1 1,-1 1-1,0 0 1,0 0-1,-1 1 1,1-1-1,-1 1 1,0 0-1,-1 0 1,1 0-1,-1 1 1,0-1-1,0 1 0,0 0 1,-1 0-1,0 0 1,0 0-1,-1 0 1,0 1-1,0-1 1,0 0-1,-1 1 1,0-1-1,0 0 1,0 1-1,-1-1 1,0 0-1,-1 5 25,-1-4 14,0-1 0,0 1 0,0-1 0,-1 1 0,1-1 0,-2 0 0,1-1 0,-1 1 0,1-1 0,-2 1 0,1-2 1,0 1-1,-7 4-14,9-7 20,0 0 1,0 0 0,-1 0-1,1 0 1,0-1 0,-1 1-1,1-1 1,-1 0 0,1 0 0,-1 0-1,0 0 1,1-1 0,-1 1-1,0-1 1,0 0 0,1 0-1,-1 0 1,0-1 0,0 0-1,1 1 1,-1-1 0,0 0 0,1-1-1,-1 1 1,1-1 0,0 1-1,-3-3-20,1 0 32,0 0-1,0 0 0,0-1 0,1 0 1,0 0-1,0 0 0,0-1 1,1 1-1,0-1 0,0 0 0,0 0 1,0 0-1,1 0 0,0 0 0,1-1 1,-1 1-1,1-1 0,0 1 1,1-1-1,0 1 0,0-1 0,1-6-31,1 9-27,0 0 0,0 1 0,0-1 0,1 0 0,-1 1 0,1-1 0,0 1 0,0 0 0,0 0 0,1 0 0,-1 1 0,1-1 0,0 1 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,1 1 0,-1 0 0,0 0 0,0 0 0,1 1 0,-1-1 0,1 1 0,-1 0 0,0 0 0,1 1 0,-1-1 0,0 1 0,1 0 0,-1 0 0,0 0 0,0 1 0,0 0 0,0-1 0,0 1 0,0 1 0,0-1 0,-1 1 0,1-1 0,-1 1 0,0 0 0,1 0 0,-1 0 0,1 3 27,-3 0-27,0 0 0,0-1 1,-1 1-1,0 0 0,0 0 1,0 0-1,-1 0 0,0 0 1,0-1-1,-1 1 0,1 0 1,-1-1-1,-1 1 0,1-1 1,-1 1-1,0-1 0,0 0 1,0 0-1,0-1 0,-1 1 1,0-1-1,-1 1 27,-2 4 70,-1-1 0,0 0 0,0 0 0,-1-1 0,0 0 0,0-1 0,-1 1 0,0-2 0,0 0 0,0 0 0,-2 0-70,7-3 34,0 0 1,-1-1-1,1 1 0,0-1 1,0 0-1,-1-1 0,1 1 1,-1-1-1,1 0 1,0 0-1,-1-1 0,1 0 1,-1 0-1,1 0 0,0 0 1,0-1-1,0 0 0,0 0 1,0 0-1,0-1 1,0 0-1,1 0 0,0 0 1,-3-2-35,3 1 33,0-1 0,1 1 1,-1-1-1,1 0 1,0 0-1,1 0 0,-1 0 1,1-1-1,0 1 1,0-1-1,0 1 0,1-1 1,0 0-1,0 0 1,1 1-1,0-1 0,0 0 1,0 0-1,0 0 0,1 1 1,0-1-1,0 0 1,2-5-34,-3 10-3,0 0 1,1 0 0,-1 0 0,0 0-1,0 0 1,1 0 0,-1 0 0,0 1-1,1-1 1,-1 0 0,1 0 0,-1 0-1,1 0 1,-1 0 0,1 1 0,0-1-1,0 0 1,-1 0 0,1 1 0,0-1-1,0 1 1,0-1 0,-1 1 0,1-1-1,0 1 1,0-1 0,0 1 0,0 0-1,0-1 1,0 1 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,1 1 3,31 26-323,-29-22 305,0 1 0,0 0 0,0 0 0,-1 0 0,1 0 1,-2 1-1,1 0 0,-1-1 0,0 1 0,0 0 0,-1 0 0,0 0 1,0 0-1,0 0 0,-1 0 0,0 0 0,-1 1 0,0-1 0,0 0 1,0 0-1,-1 0 0,0-1 0,-2 7 18,3-12 21,1 0 1,0 0-1,0 0 1,-1 0-1,1 1 1,-1-1-1,1 0 0,-1 0 1,0 0-1,1 0 1,-1-1-1,0 1 1,0 0-1,1 0 1,-1 0-1,0 0 0,0-1 1,0 1-1,0 0 1,0-1-1,0 1 1,0-1-1,0 1 0,-1-1 1,1 0-1,0 1 1,0-1-1,0 0 1,0 0-1,0 0 0,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,-1-1 1,1 1-1,0 0 0,0-1 1,0 1-1,0-1 1,0 1-1,0-1 1,0 0-1,0 1 0,0-1 1,0 0-1,0 0 1,1 1-1,-1-1 1,-1-1-22,-3-7 29,-1-1-1,2 0 1,-1 0 0,1 0 0,1-1 0,0 1 0,0-1 0,1 0 0,0 0 0,1 0 0,0 0 0,1 0 0,0 0-1,1 0 1,0 0 0,2-4-29,-3 3 18,0 8-14,0-1 1,0 0 0,0 1 0,1-1 0,0 1 0,-1-1-1,1 0 1,1 1 0,-1 0 0,1-1 0,0 1 0,0 0-1,0 0 1,0 0 0,1 0 0,0 0 0,0 0 0,0 1-1,0-1 1,0 1 0,1 0 0,-1 0 0,1 0 0,0 1-1,0-1 1,0 1 0,0 0 0,0 0 0,1 0 0,-1 1-1,0-1 1,2 1-5,-2 0-24,1 0-1,-1 1 1,1-1 0,0 1-1,-1 0 1,1 1-1,-1-1 1,1 1 0,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 1 0,0 0-1,0 0 1,0 0-1,0 0 1,0 1 0,0-1-1,-1 1 1,1 0-1,-1 0 1,0 1 0,0-1-1,0 0 1,0 1-1,0 0 1,-1 0 0,0 0-1,0 0 1,0 0-1,0 0 1,-1 1 0,1-1-1,-1 0 1,0 1-1,-1-1 1,1 1 0,-1-1-1,1 1 25,-4 3 5,0 0 1,0 0-1,0-1 0,-1 0 0,0 0 0,0 0 0,-1 0 0,0 0 1,0-1-1,0 0 0,-1 0 0,0-1 0,0 1 0,-1-1 0,0-1 0,1 1 1,-1-1-1,-1 0 0,1-1 0,-1 1 0,1-2 0,-1 1 0,0-1 1,0 0-1,0-1 0,0 1 0,-8-1-5,13-2 12,-1 1 1,1 0-1,-1-1 0,1 0 1,-1 0-1,1 0 0,0 0 1,0-1-1,-1 1 1,1-1-1,0 0 0,0 0 1,1 0-1,-1 0 0,0 0 1,1-1-1,-1 1 0,1-1 1,0 0-1,0 1 0,0-1 1,0 0-1,0 0 1,1-1-1,-1 1 0,1 0 1,0 0-1,0-1 0,0 1 1,0-1-1,1 1 0,-1-1 1,1 1-1,0-1 0,0 1 1,0-1-1,0 1 1,1-1-1,0 1 0,0 0 1,0-3-13,0 4 5,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,1 1-1,-1-1 1,1 0 0,-1 1-1,1-1 1,0 1-1,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0 1 0,0-1-1,0 0 1,0 1-1,0-1 1,1 1-1,-1-1 1,0 1-1,0 0 1,1 0-1,-1 0 1,0 0 0,0 1-1,1-1 1,-1 0-1,0 1 1,0 0-1,0-1 1,0 1-1,0 0 1,0 0 0,0 0-1,0 1 1,0-1-1,0 0 1,0 1-1,-1-1 1,1 1-1,-1 0 1,1-1-1,-1 1 1,0 0 0,1 0-6,1 1 10,0 0 0,0 1 0,-1-1 1,1 1-1,-1-1 0,0 1 0,0 0 0,0 0 1,0 0-1,-1 0 0,1 0 0,-1 1 1,0-1-1,-1 0 0,1 1 0,-1-1 1,1 0-1,-2 1 0,1-1 0,0 0 1,-1 1-1,1-1 0,-1 0 0,-1 0 0,1 1 1,0-1-1,-1 0 0,0 0 0,0 0 1,0-1-1,0 1 0,-1 0 0,0-1 1,1 0-1,-1 1 0,-1-1 0,1 0-10,1-2-4,1 0-1,-1 0 0,0 0 0,1-1 1,-1 1-1,0-1 0,0 1 0,0-1 1,0 1-1,0-1 0,0 0 0,1 0 1,-1 0-1,0 0 0,0 0 0,0-1 1,0 1-1,0 0 0,0-1 0,0 1 1,1-1-1,-1 0 0,0 0 0,1 0 1,-1 0-1,0 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,1-1 1,0 1-1,0-1 0,-1 1 0,1-1 1,0 0-1,0-1 5,-1 1-265,0 0 0,1 0 0,0 0 0,-1 0 0,1-1 0,0 1 0,0-1 1,0 1-1,1-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,0 0 0,0 1 0,0-1 1,0 0-1,0 1 0,1-1 0,-1 1 0,1-1 0,0 1 0,-1-1 0,1 1 0,1-1 0,-1 1 1,1-2 264,7-3-672</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink26.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-06-24T04:06:41.022"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#66CC00"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">175 186 8064,'0'0'2672,"0"4"2400,7-5-4745,-6 1-315,0-1 0,0 1 0,-1-1 0,1 1 0,0 0 0,0-1 0,0 1-1,0 0 1,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,0 0 0,0-1 0,-1 1 0,1 0 0,-1 0 0,1 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,-1 0-12,-1 3 172,0-1 1,0 1-1,-1-1 0,1 1 0,-1-1 1,0 0-1,0 0 0,0 0 1,-1-1-1,1 1 0,0-1 0,-1 0 1,0 0-1,0 0 0,1 0 0,-1-1 1,0 1-1,-1-1 0,1 0 0,-2 0-172,4-2 37,0 0-1,1 0 0,-1-1 0,0 1 0,1 0 0,0-1 1,-1 1-1,1-1 0,0 0 0,0 1 0,0-1 1,0 0-1,0 0 0,0 0 0,0 0 0,1 0 0,-1 1 1,1-1-1,-1-1 0,1 1 0,0 0 0,-1 0 0,1 0 1,1 0-1,-1 0 0,0 0 0,0 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,1 0-36,0 0 0,-1-4-4,1 1 1,-1-1-1,1 0 1,1 1-1,-1-1 1,1 1 0,0 0-1,1-1 1,-1 1-1,1 0 1,0 0-1,0 1 1,0-1 0,1 1-1,0-1 1,0 1-1,0 0 1,0 0-1,1 1 1,-1-1-1,1 1 1,0 0 0,0 1-1,0-1 1,0 1-1,0 0 1,1 0-1,-1 0 1,1 1-1,0 0 1,-1 0 3,-4 1-9,0 0 1,1 0-1,-1 0 0,0 0 0,0 0 1,0 1-1,0-1 0,0 0 1,0 1-1,0-1 0,0 0 0,0 1 1,0 0-1,0-1 0,0 1 1,0-1-1,-1 1 0,1 0 0,0 0 1,0 0-1,-1-1 0,1 1 0,0 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 1,1 0-1,-1 1 0,0-1 0,0 0 1,0 0-1,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,-1 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,1 0 1,-1 0-1,0 0 0,1-1 1,-1 1-1,0 0 0,0 0 0,0-1 1,0 1-1,0 0 0,0-1 0,0 1 1,0-1 8,-1 3 30,0 0 1,-1-1-1,0 1 0,1-1 1,-1 1-1,0-1 1,0 0-1,-1 0 0,1-1 1,0 1-1,-1 0 1,1-1-1,-1 0 0,1 0 1,-1 0-1,1 0 1,-1-1-1,0 1 1,1-1-1,-1 0 0,0 0 1,0 0-1,1-1 1,-1 1-1,0-1 0,1 0 1,-1 0-1,1 0 1,-1-1-1,1 1 0,0-1 1,-1 0-1,1 0 1,0 0-1,0 0 1,0 0-1,1-1 0,-1 1 1,0-1-1,1 0 1,0 0-1,-1 0 0,1 0 1,1 0-1,-1 0 1,0-1-1,1 1-30,-1 0 10,1-1 1,0 1-1,0 0 1,0-1-1,1 1 1,-1-1-1,1 1 1,0-1-1,0 1 1,0-1-1,0 1 1,1 0-1,0-1 1,-1 1-1,1-1 1,0 1-1,1 0 1,-1 0-1,0 0 1,1-1-1,0 1 1,0 1-1,0-1 1,0 0-1,0 0 1,0 1-1,1-1 1,-1 1-1,1 0 1,0 0-1,3-2-10,-5 3-15,1 1-1,0-1 1,0 1-1,-1-1 1,1 1-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0-1,0 0 1,0 0-1,-1 0 1,1 1-1,0-1 1,0 1-1,-1 0 1,1-1-1,0 1 1,-1 0-1,1 0 1,-1 0 0,1 0-1,-1 0 1,1 0-1,-1 0 1,0 1-1,0-1 1,0 1-1,1-1 1,-1 0-1,0 2 16,28 52-598,-28-48 604,1 0-1,-1 0 1,0 1-1,-1-1 1,0 0-1,0 0 1,0 0-1,-1 0 1,0 0-1,-1 0 1,1 0-1,-1 0 1,-1 0-1,1 0 1,-1-1-1,0 1 1,-1-1-1,0 0 1,0 0-1,0 0 1,0-1-1,-1 1 1,0-1-1,0 0 1,-1-1-1,1 1 1,-1-1-1,0 0 1,0 0-1,0-1 1,-6 3-6,9-6 10,1 0 1,-1 1-1,0-1 1,1 0-1,-1 0 1,0-1-1,1 1 1,-1 0-1,1-1 1,-1 0-1,0 0 1,1 1 0,-1-2-1,1 1 1,0 0-1,-1 0 1,1-1-1,0 1 1,0-1-1,0 0 1,0 1-1,0-1 1,0 0-1,0 0 1,1-1-1,-1 1 1,1 0-1,-1 0 1,1-1-1,0 1 1,0-1-1,0 1 1,0-1 0,1 1-1,-1-1 1,1 0-1,-1 1 1,1-3-11,-1 2-4,0-1 1,1 1 0,-1 0 0,1-1 0,0 1 0,0 0-1,0-1 1,0 1 0,1 0 0,-1 0 0,1-1 0,0 1-1,0 0 1,0 0 0,0 0 0,0 0 0,1 0 0,-1 0-1,1 0 1,0 0 0,0 0 0,0 1 0,0-1-1,1 1 1,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0-1,0 0 1,0 0 0,0 1 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,1 0 0,-1 1 0,0-1 0,1 1-1,2 0 4,-2 1-37,1 0 0,-1 1 0,0-1 0,0 1 0,0 0 0,1 0 0,-2 0 1,1 0-1,0 1 0,0-1 0,-1 1 0,1 0 0,-1 0 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,0 1 0,0-1 0,0 1 0,0-1 0,-1 1 0,1-1 0,-1 1 0,0-1 0,-1 1 0,1-1 0,-1 1 0,0-1 0,0 0 0,0 1 0,-1-1 0,1 0 0,-1 0 0,0 0 0,0 0 0,-1 0 0,-1 3 37,1-4 66,0 0 0,0 1 0,0-1 0,0 0 0,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 1 0,0-1 0,0 0 0,0-1 0,0 1 0,-1-1 0,1 0 0,-4 1-66,3-3 39,-1 0 1,1 0-1,0-1 0,0 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,1-1 0,-1 0 1,1 0-1,0-1 0,0 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,1-1 0,0 1 1,1-1-1,-1 0 0,1 0 0,0 1 0,0-1 0,1-1 0,-1 1 0,1 0 0,0 0 1,1 0-1,-1-1 0,1 1 0,0 0 0,0-1 0,1 1 0,-1 0 0,1 0 0,1-1 1,-1 1-1,1-1-39,-1 1-3,0 1 0,0 0 0,1 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,1 0 0,-1 1 1,1-1-1,0 1 0,0 0 0,0 0 0,0 0 1,0 0-1,1 0 0,-1 0 0,1 1 0,1-1 3,3 1-52,1 1 0,-1 0 1,1 1-1,-1 0 0,1 0 0,-1 0 0,1 1 0,-1 1 0,0-1 0,1 2 0,-1-1 0,0 1 0,0 0 0,0 0 0,-1 1 0,1 0 1,-1 1-1,0-1 0,2 3 52,-6-5-13,0-1 0,0 1 0,0-1 1,0 1-1,0 0 0,0 0 0,-1 1 1,1-1-1,-1 0 0,1 1 1,-1-1-1,0 1 0,0 0 0,0 0 1,-1 0-1,1 0 0,-1 0 0,1 0 1,-1 1-1,0-1 0,0 0 0,0 0 1,-1 1-1,1-1 0,-1 1 0,0-1 1,0 1-1,0-1 0,-1 0 0,1 1 1,-1-1-1,1 1 0,-1-1 1,0 0-1,0 0 0,-1 2 13,-5 1 16,1 0-1,-1-1 1,0 0 0,-1 0 0,1-1-1,-1 0 1,0 0 0,0 0 0,0-1-1,-1 0 1,1-1 0,-1 0 0,1 0-1,-1-1 1,0 0 0,0-1-1,1 0 1,-1 0 0,0-1 0,0 0-16,2 1 35,0 0 1,0-1-1,0 0 0,0 0 1,0 0-1,0-1 1,0 0-1,0-1 1,1 1-1,-1-1 1,-1-2-36,5 4 21,1-1 1,0 1 0,0-1 0,-1 0 0,1 0 0,0 0 0,1 0 0,-1 0-1,0-1 1,1 1 0,-1 0 0,1-1 0,-1 1 0,1-1 0,0 1-1,0-1 1,0 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 0-1,0 1 1,0-1 0,0 0 0,1 0 0,-1 0 0,1 1 0,-1-1-22,1 0 7,-1 0 0,1 0 1,0 0-1,0 0 1,0 1-1,1-1 0,-1 0 1,1 1-1,-1-1 1,1 1-1,0-1 0,0 1 1,0 0-1,0 0 1,0-1-1,1 2 0,-1-1 1,0 0-1,1 0 1,0 1-1,-1 0 0,1-1 1,0 1-1,0 0 1,0 0-1,-1 0 0,1 1 1,0-1-1,0 1 1,0 0-1,1 0-7,5 0-79,0 0 0,-1 1 0,1 1 0,0-1 0,0 1 0,-1 1 0,1 0 0,-1 0 0,0 0 0,0 1 0,0 1 0,0-1 0,-1 1 0,0 0 0,0 1 0,6 5 79,-11-7-12,0-1-1,0 0 1,-1 1 0,1-1-1,-1 1 1,1 0 0,-1-1-1,0 1 1,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0-1,0-1 1,-1 1 0,1 0-1,-1 0 1,1 0-1,-1 0 1,-1-1 0,1 1-1,0 0 1,-1-1 0,0 1-1,1-1 1,-1 0 0,-1 1-1,1-1 1,0 0 0,-1 0-1,0 0 1,1-1 0,-1 1-1,0-1 1,-3 2 12,3-3 28,1 1 1,-1-1-1,0 0 0,0 0 1,0 0-1,-1 0 0,1-1 1,0 1-1,0-1 0,0 0 1,0 0-1,0 0 0,-1 0 0,1-1 1,0 1-1,0-1 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0-1 0,1 1 1,-1-1-1,0 0 0,1 0 1,-1 0-1,1 0 0,0 0 1,0 0-1,0-1 0,0 1 1,0-1-1,0 1 0,1-1 0,-1 0 1,1 0-1,0 0 0,-1 0 1,1 0-1,1 0 0,-1-2-28,-3-3 22,1 0 0,0 0-1,0-1 1,1 1-1,0-1 1,1 0 0,0 0-1,0 0 1,1 1-1,0-1 1,1 0 0,0 0-1,0 0 1,1 1-1,0-1 1,0 0 0,1 1-1,0 0 1,1-1-1,3-5-21,-4 11-3,1 0 0,-1 0 1,0 0-1,1 0 0,-1 1 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 1,0 1-1,1 0 0,-1 1 0,0-1 0,1 1 0,-1 0 0,0 0 0,1 0 0,-1 1 0,4 0 3,1-1-37,1 0 0,-1 1-1,0 0 1,0 1 0,0 0-1,0 0 1,0 1 0,0 0-1,-1 1 1,1 0 0,-1 0-1,0 0 1,0 1 0,-1 1-1,1-1 1,-1 1 0,0 1-1,0 0 38,-6-6-1,1 1-1,-1 0 0,0 0 0,0-1 1,0 1-1,0 0 0,0 0 0,0 0 1,-1 0-1,1 0 0,-1 0 0,1 0 1,-1 0-1,0 0 0,0 0 0,0 0 1,0 1-1,0-1 0,0 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,0 0 1,0 0-1,1 0 0,-1 0 0,0 0 1,0-1-1,-1 1 0,1 0 0,0-1 1,-1 1-1,1-1 0,-2 2 2,-66 41 211,58-40-150,1-1 1,-1 0 0,0-1 0,1 0-1,-1 0 1,0-1 0,0-1-1,0 0 1,0 0 0,0-1-1,0-1 1,0 0 0,0 0 0,0-1-62,8 2 13,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,1-1 1,-1 1-1,1-1 1,-1 0 0,1 1-1,0-1 1,-1 0-1,1-1 1,0 1 0,0 0-1,0 0 1,1-1-1,-1 0 1,1 1 0,-1-1-1,1 0 1,0 1-1,0-1 1,0 0 0,0 0-1,1 0 1,-1 0-1,1 0 1,0 0 0,-1 0-1,1 0 1,1 0-1,-1 0 1,0 0 0,1 0-1,0 0 1,-1 0-1,1 0 1,0 1 0,1-2-14,1 2-3,-1-1 0,1 1 0,0 0 0,0 0 0,0 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,1 0 0,-1 0 0,0 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1 0 0,0 1 0,-1-1 0,1 0 0,-1 1 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 1 0,-1-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,2 2 3,-2-2-89,-1-1-1,1 1 1,-1-1-1,0 1 1,0 0 0,0 0-1,0-1 1,0 1-1,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,-1 0 0,0 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,-1 0 1,1 0-1,0 1 1,0-1-1,-1 0 1,0 0 0,1-1-1,-1 1 1,0 0-1,0 0 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,-1-1 1,1 1 0,-1-1-1,1 0 1,-1 1-1,0-1 1,1 0-1,-1 0 1,0 0-1,-1 1 90,-10-2-1189,-4-10 554</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink27.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-06-24T04:06:41.023"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#849398"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">74 193 4224,'-24'-11'7984,"11"-29"-4725,9 20-2220,0-49 726,4 68-1764,0 1 0,0-1 0,0 0-1,0 1 1,0-1 0,1 1-1,-1-1 1,0 1 0,0-1-1,0 1 1,0-1 0,1 0-1,-1 1 1,0-1 0,1 1 0,-1 0-1,0-1 1,1 1 0,-1-1-1,0 1 1,1-1 0,-1 1-1,1 0 1,-1-1 0,1 1-1,-1 0 1,1 0 0,-1-1-1,1 1 1,-1 0 0,1 0 0,0 0-1,-1-1 1,1 1 0,-1 0-1,1 0 1,-1 0 0,1 0-1,0 0 1,-1 0 0,1 0-1,-1 0 1,1 1 0,-1-1 0,1 0-1,-1 0 1,1 0 0,0 1-1,-1-1 0,30 14 9,-24-11-46,0 0 0,-1 1 0,1 0 0,-1 0 0,0 1 0,0-1 0,0 1 0,-1 0 1,1 0-1,-1 1 0,-1-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,0 0 0,-1 1 0,0-1 0,0 1 0,-1-1 0,0 1 0,0-1 0,-1 1 0,1 0 0,-1 0 0,-1-1 0,1 1 0,-3 6 37,3-10 24,-1 1-1,0-1 1,0 0-1,0 1 0,-1-1 1,1 0-1,-1 0 0,0 0 1,1 0-1,-1 0 0,-1-1 1,1 1-1,0 0 0,-1-1 1,1 0-1,-1 1 0,0-1 1,0 0-1,0-1 0,0 1 1,0 0-1,0-1 1,0 0-1,0 1 0,-1-1 1,1-1-1,0 1 0,-1 0 1,1-1-1,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 1,1-1-1,-1 1 0,-2-2-23,1-3 43,0 0 0,0-1 0,0 1 0,1-1 0,0 0 0,0 0-1,1-1 1,0 1 0,0-1 0,0 0 0,1 0 0,0 1 0,0-2 0,0 1-1,1 0 1,1 0 0,-1 0 0,1-1 0,0 1 0,0 0 0,1 0-1,0 0 1,1-1 0,-1 1 0,1 0 0,1 1 0,1-6-43,-3 9-2,-1 1 1,1 0 0,0-1 0,-1 1-1,1-1 1,0 1 0,0 0 0,0-1-1,1 1 1,-1 0 0,1 0 0,-1 0-1,1 0 1,0 0 0,-1 0 0,1 1-1,0-1 1,0 1 0,0-1-1,1 1 1,-1 0 0,0-1 0,0 1-1,1 0 1,-1 1 0,0-1 0,1 0-1,-1 1 1,1-1 0,-1 1 0,1 0-1,0 0 1,-1 0 0,1 0 0,-1 0-1,1 1 1,-1-1 0,1 1 1,3 3-14,-1 0 0,-1 1 0,1 0 0,-1 0 0,1 0 0,-1 1 0,-1-1 0,1 1 0,-1 0-1,0 0 1,-1 0 0,1 1 0,-1-1 0,0 1 0,-1-1 0,1 1 0,-1-1 0,-1 1 0,1 0 0,-1-1 0,0 1 0,-1 0 0,0 0 0,0-1 0,0 1 0,-1-1 0,-1 4 14,2-5 16,0 0-1,-1 0 0,0 0 1,0 0-1,0 0 1,-1 0-1,1-1 1,-1 1-1,0-1 0,-1 0 1,1 0-1,-1 0 1,1 0-1,-1-1 1,0 0-1,0 1 1,-1-1-1,1-1 0,-2 1-15,5-2 15,0-1 0,0 0-1,0 0 1,-1-1 0,1 1-1,0 0 1,0 0 0,0-1-1,0 1 1,0 0 0,0-1 0,-1 1-1,1-1 1,0 1 0,0-1-1,1 0 1,-1 1 0,0-1-1,0 0 1,0 0 0,0 0-1,0 0 1,1 0 0,-1 0-1,1 0 1,-1 0 0,0 0-1,1 0 1,-1 0 0,1 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,0-1 0,0 1-1,0 0-14,-3-51 193,4 47-177,0 0-1,1 0 0,-1 1 0,1-1 0,0 1 0,0-1 1,0 1-1,1 0 0,0 0 0,-1 0 0,1 0 0,1 0 1,-1 0-1,1 1 0,-1 0 0,1 0 0,0 0 0,0 0 1,0 0-1,1 1 0,-1 0 0,0 0 0,1 0 0,0 0 1,-1 1-1,1 0 0,0 0 0,0 0 0,0 1 0,0-1 1,0 1-1,4 0-15,-6 1-4,0-1 1,0 1 0,0 0-1,0 0 1,0 0 0,0 0-1,0 1 1,0-1-1,0 1 1,-1 0 0,1-1-1,-1 1 1,1 0 0,-1 1-1,0-1 1,0 0 0,0 1-1,0-1 1,0 1-1,0-1 1,-1 1 0,1 0-1,-1 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,-1 0 1,0 0-1,1 0 1,-1 1 0,0-1-1,0 0 1,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0-1,0 0 1,0 0-1,-1 0 1,1 0 0,-1 0-1,1 0 1,-2 1 3,-1 2 82,0 0 0,-1 0 0,0 0-1,0-1 1,0 1 0,-1-1 0,0 0 0,0-1 0,0 0 0,0 0-1,-1 0 1,1 0 0,-1-1 0,0 0 0,0-1 0,0 0 0,-1 0-1,1 0 1,0-1 0,-1 0 0,1 0 0,-1-1 0,0 0-82,5-2 11,0 0 0,-1 0 0,1 0 0,1 0 1,-1 0-1,0-1 0,0 1 0,1-1 0,-1 0 0,1 0 1,0 0-1,0 0 0,0 0 0,1 0 0,-1-1 1,1 1-1,-1 0 0,1-1 0,0 1 0,0-1 1,1 0-1,-1 1 0,1-1 0,0 0 0,0 1 0,0-1 1,0 0-1,0 1 0,1-1 0,0 0 0,0 0-11,0-2-2,-1 1 0,1 0 0,0 0 0,1 0 0,-1-1 0,1 1-1,0 1 1,0-1 0,1 0 0,-1 0 0,1 1 0,0 0 0,0-1-1,1 1 1,-1 0 0,1 1 0,0-1 0,0 1 0,0-1 0,1 1 0,-1 0-1,1 1 1,-1-1 0,1 1 0,1 0 2,-2 0-7,0 1 1,0-1-1,0 2 1,0-1-1,0 0 1,0 1-1,0-1 0,1 1 1,-1 0-1,0 1 1,0-1-1,0 1 1,0-1-1,0 1 1,0 1-1,0-1 0,0 0 1,0 1-1,0 0 1,-1 0-1,1 0 1,-1 0-1,1 1 0,-1 0 1,0-1-1,0 1 1,0 0-1,0 0 1,-1 0-1,1 1 0,-1-1 1,0 1-1,0-1 1,0 1-1,0 0 1,-1 0-1,0 0 1,1 0-1,-1 2 7,-2 0 25,0 0 1,0 0 0,-1 0-1,1 0 1,-1 0-1,-1-1 1,1 1-1,-1-1 1,0 1-1,0-1 1,-1 0-1,1 0 1,-1 0-1,-1 0 1,1-1-1,0 0 1,-1 0-1,0 0 1,0 0-1,0-1 1,0 0-1,-1 0 1,-1 0-26,6-2 14,0 0 1,-1 0-1,1 0 1,-1-1-1,1 1 1,-1-1-1,1 1 1,-1-1 0,0 1-1,1-1 1,-1 0-1,1 0 1,-1 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,1 0 1,-1-1 0,1 1-1,-1-1 1,1 1-1,-1-1 1,1 0-1,-1 0 1,1 1-1,-1-1 1,1 0-1,0 0 1,0 0 0,-1 0-1,1-1 1,0 1-1,0 0 1,0 0-1,0-1 1,0 1-1,1-1 1,-1 1-1,0 0 1,1-1 0,-1 0-1,0 1 1,1-1-1,-1-1-14,-5-77 119,26-9-350,-18 86 194,-1 0 0,1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 1 0,1-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,1 1-1,-1-1 1,0 1 0,1 0 0,-1-1 0,1 2 0,-1-1 0,1 0 0,3 1 37,-1-1-38,-1 1 0,1 1-1,-1-1 1,1 1 0,-1 0-1,0 0 1,1 0-1,-1 1 1,0 0 0,0 0-1,0 0 1,0 1 0,0 0-1,0 0 1,-1 0 0,1 0-1,-1 1 1,0 0 0,0-1-1,0 2 1,-1-1-1,1 0 1,-1 1 0,0-1-1,0 1 1,1 3 38,-5-2 21,1-1 0,-1 0-1,0 0 1,0 0 0,-1 0 0,1 0-1,-1 0 1,0-1 0,0 1 0,-1-1-1,0 1 1,1-1 0,-1 0 0,-1 0-1,1 0 1,-1 0 0,1 0 0,-1-1-1,0 0 1,0 0 0,-1 0 0,1 0 0,-1-1-1,1 1 1,-1-1 0,0 0 0,0-1-1,-1 1-20,3 0 16,0 0 0,0 0 0,-1-1 0,1 0 0,0 1 0,-1-1 0,1 0 0,-1-1 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 0 0,1 0 0,-1-1 0,0 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1-1 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1-1 0,-1 1 0,1-1 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,1-2-16,0 4-8,1-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,1 0 0,-1-1 0,0 1 0,1-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,-1 0 0,1-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,1 0 0,-1 1 0,0-1 0,1 0 0,-1 1 0,0-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,0 0 0,1 0 0,-1 0 0,1 0 8,58 7-473,-58-6 443,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,-1 1-1,1-1 1,0 1 0,-1-1-1,1 1 1,-1 0 0,0 0-1,0-1 1,1 1 0,-1 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,0 1 0,-1-1 29,-1 3 16,0 0 1,0 0-1,-1 0 1,0 0-1,0 0 0,0 0 1,0 0-1,-1-1 1,0 1-1,0-1 1,0 0-1,-1 0 1,1 0-1,-1 0 1,0-1-1,0 1 1,0-1-1,0 0 0,-1 0 1,1-1-1,-1 1 1,0-1-1,0 0-16,2 0 27,0-1-1,0 0 0,-1 0 0,1 0 1,0 0-1,-1 0 0,1-1 0,-1 1 1,1-1-1,-1 0 0,1 0 1,-1 0-1,1-1 0,-1 1 0,1-1 1,-1 0-1,1 0 0,0 0 0,0 0 1,-1-1-1,1 1 0,0-1 0,0 0 1,0 0-1,0 0 0,1 0 0,-1 0 1,1-1-1,-1 1 0,1-1 1,0 0-1,0 1 0,0-1 0,0 0 1,0 0-1,1 0 0,-1-1 0,1 1 1,0 0-1,0-2-26,-2 0 1,1-1 0,0 0 0,0 1 0,0-1 0,1 0 0,0 0 0,0 0 1,1-1-1,0 1 0,0 0 0,0 0 0,0 0 0,1 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,1 1 0,-1-1 0,1 1 0,0 0 1,1-1-1,-1 1 0,2 0-1,-1 2-13,1 1 1,-1 0 0,1 1-1,0-1 1,0 1 0,0 0 0,0 0-1,0 0 1,0 1 0,0 0-1,0 0 1,0 0 0,0 0 0,0 1-1,1 0 1,-2 0 0,1 0-1,0 1 1,0 0 0,0 0 0,-1 0-1,1 0 1,-1 1 12,0-2-3,-1 0 1,0 0-1,1 0 0,-1 1 1,0 0-1,0-1 0,0 1 1,-1 0-1,1 0 0,0 1 1,-1-1-1,1 0 0,-1 1 1,0 0-1,0-1 0,0 1 1,0 0-1,0 0 0,0 0 1,-1 0-1,0 1 0,0-1 1,0 0-1,0 1 0,0-1 1,0 0-1,-1 1 0,0-1 1,0 1-1,0-1 0,0 1 1,0-1-1,-1 1 0,1-1 1,-1 0-1,0 1 0,0-1 1,0 0-1,0 0 0,-1 1 1,0-1-1,1 0 0,-1 0 1,-2 2 2,2-2 25,0 0 1,0-1 0,0 1 0,0 0-1,0-1 1,-1 1 0,1-1-1,-1 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0-1 0,0 1 0,0-1-1,0 0 1,-1 0 0,1 0-1,0 0 1,-1-1 0,1 1 0,-1-1-1,1 0 1,-1 0 0,1 0-1,0 0 1,-1-1 0,1 1 0,-1-1-1,1 0 1,0 0 0,-1 0 0,1-1-1,-1 0-25,-1-5 4,1 0 0,0 0 0,1 0 0,-1-1 0,2 1 0,-1-1 0,1 0 0,0 0 0,0 0 0,1 0 0,0 0 0,1 0 0,0 0-1,0-1 1,1 1 0,0 0 0,0 0 0,0 0 0,1 0 0,1 0 0,-1 1 0,1-1 0,2-1-4,-3 3 6,1-1 0,1 1 0,-1 0 0,1 0 0,0 0 0,0 1 0,1 0 0,0-1 0,0 1 0,0 0-6,-3 4-6,0 0 0,-1 0 0,1-1 0,0 1 1,0 0-1,0 0 0,0 1 0,0-1 0,0 0 0,0 1 1,0-1-1,0 1 0,0 0 0,0-1 0,0 1 0,0 0 1,0 0-1,0 1 0,0-1 0,1 0 0,-1 1 0,0-1 1,0 1-1,0-1 0,0 1 0,-1 0 0,1 0 0,0 0 0,0 0 1,0 0-1,-1 1 0,1-1 0,-1 1 0,1-1 6,3 4-3,0 0 1,0 0-1,-1 0 0,0 0 0,0 1 0,0-1 0,-1 1 1,1 0-1,-2 0 0,1 1 0,-1-1 0,1 0 0,-2 1 1,1 0-1,-1-1 0,0 1 0,0 0 0,-1-1 0,0 1 1,0 0-1,-1 0 0,0-1 0,0 1 0,0 0 0,-1-1 1,0 1-1,0-1 0,-1 0 0,0 1 0,0-1 0,0-1 1,-4 6 2,1-4 32,0 0 0,0 0 1,-1 0-1,1-1 0,-2 0 0,1 0 1,-1-1-1,0 1 0,0-2 1,0 1-1,-1-1 0,1-1 0,-1 0 1,0 0-1,0 0 0,0-1 1,0-1-1,-7 1-32,14-2 4,-1 0-1,1 0 1,-1 0 0,1 0 0,-1 0-1,1-1 1,0 1 0,-1-1 0,1 0-1,-1 1 1,1-1 0,0 0-1,0-1 1,0 1 0,-1 0 0,1-1-1,0 1 1,1-1 0,-1 1 0,0-1-1,0 0 1,1 0 0,-1 0 0,1 0-1,-1 0 1,1 0 0,0 0-1,0-1 1,0 1 0,0 0 0,0-1-1,1 1 1,-1-1 0,1 1 0,0-1-1,-1 1 1,1-1 0,0 1 0,0 0-1,1-3-3,0 2-5,0 0 0,0 1-1,0-1 1,0 1 0,1-1-1,-1 1 1,1 0 0,0-1-1,-1 1 1,1 0 0,0 0-1,0 0 1,1 0 0,-1 0-1,0 1 1,1-1 0,-1 1-1,1 0 1,-1-1 0,1 1-1,-1 0 1,1 0 0,0 1-1,0-1 1,0 1 0,-1-1-1,1 1 1,0 0 0,0 0-1,0 0 1,0 0 0,-1 1-1,3-1 6,-1 0-5,1 0-1,-1 0 0,0 0 1,1 0-1,-1 1 1,0-1-1,0 1 0,0 0 1,0 1-1,1-1 1,-2 1-1,1-1 0,0 1 1,0 0-1,0 1 1,-1-1-1,1 1 0,-1-1 1,0 1-1,0 0 1,0 0-1,0 1 0,-1-1 1,1 0-1,-1 1 1,0 0-1,1 0 0,-2-1 1,1 1-1,0 0 1,-1 0-1,0 1 1,0-1-1,0 0 0,-1 0 1,1 0-1,-1 1 1,0-1-1,0 0 0,0 1 6,-1-1 55,0 0 0,1 0 0,-2 0 0,1 0 0,0-1 0,-1 1 0,1 0 0,-1-1 0,0 1 0,0-1 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1-1 0,0 1 0,0 0-1,-1-1 1,1 0 0,0 1 0,-1-1 0,1-1 0,-2 1-55,2-3 14,1 0 0,-1 0 0,0 0 0,1-1 0,-1 1 1,1-1-1,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,1-1 0,0 1 0,-1-1 0,1 0 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 1,0 0-1,1-1-14,-3-3-1,1 0 0,0 1 0,1-1 0,0 0 0,0 1 0,0-1 0,1 0 0,0 1 0,0-1 0,1 0 0,-1 1 0,1 0 1,1-1-1,-1 1 0,1 0 0,1 0 0,-1 0 0,1 1 0,0-1 0,0 1 0,0 0 0,1 0 0,1-1 1,-5 5-16,1 1 0,0-1 1,0 0-1,0 1 0,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,-1 1 0,1 0 0,0 1 0,0-1 0,0 0 1,0 1-1,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 1,-1 0-1,1 1 0,-1-1 0,1 0 0,-1 1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 1,0 0-1,0 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,-1 0 0,1 0 0,-1 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,0-1 1,0 1-1,0 0 16,0-2-279,1 1 1,-1 0 0,1-1-1,-1 1 1,0 0 0,1-1-1,-1 1 1,1 0 0,-1-1-1,0 1 1,0-1 0,1 0-1,-1 1 1,0-1 0,0 0-1,0 1 1,1-1 0,-1 0-1,0 0 1,0 1 0,0-1-1,0 0 1,0 0 0,0 0-1,1 0 1,-1 0 0,0 0-1,0-1 1,0 1 0,0 0-1,0 0 1,1-1 0,-1 1-1,0 0 1,0-1 0,0 1-1,1-1 279,-8-15-1482</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink28.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-06-24T04:06:41.024"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#ED7D31"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">95 174 5504,'28'-58'7754,"-24"53"-7483,0 0 0,0 0-1,1 0 1,0 1 0,-1 0 0,2 0-1,-1 0 1,0 1 0,1-1 0,-1 1-1,1 0 1,0 1 0,0 0 0,0 0-1,1 0 1,-1 0 0,1 1-271,-7 1 6,1 0 0,-1 0 0,1 0 0,-1 0-1,1 0 1,-1 0 0,1 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,0 0-1,1 1 1,-1-1 0,1 0 0,-1 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,0 1 0,0-1 0,0 1-1,0-1 1,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 1-1,-1-1 1,1 1-6,-15 24-266,13-21 391,-1 0 0,0-1-1,0 0 1,0 1-1,0-1 1,-1 0-1,0-1 1,1 1-1,-1-1 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,-1-1-1,1 0 1,-1 0-125,3-1 14,1 0 0,0-1 0,-1 1 0,1-1 1,0 1-1,-1-1 0,1 1 0,0-1 0,0 0 1,-1 0-1,1 1 0,0-1 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0-1 0,1 1 1,-1 0-1,0 0 0,1-1 0,-1 1 0,1 0 1,-1 0-1,1-1 0,-1 1 0,1-1 0,0 1 0,0 0 1,0-1-1,0 1 0,0-1 0,0 1 0,0 0 1,0-1-1,1 1 0,-1-1 0,0 1 0,1 0 1,-1-1-1,1 1 0,0 0 0,-1 0 0,1-1 1,0 1-1,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 1,1 0-1,-1 0 0,0 0 0,0 1 0,0-1 1,0 0-1,1 1 0,-1-1-14,1 0-11,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 1-1,0-1 1,0 1-1,0-1 0,0 1 1,1 0-1,-1 0 1,0 0-1,0 0 1,0 0-1,0 1 1,0-1-1,0 0 0,1 1 1,-1 0-1,0-1 1,0 1-1,0 0 1,-1 0-1,1 0 0,0 1 1,0-1-1,0 0 1,-1 1-1,1-1 1,-1 1-1,1-1 1,-1 1-1,0 0 0,1-1 1,-1 1-1,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,-1 0 0,1 0 1,-1 0-1,0 0 1,0 1-1,1-1 1,-1 0-1,-1 1 11,1 5 25,-1 0 0,-1 0 0,1 0 0,-2 0 0,1-1 0,-1 1 0,0-1 0,0 1 0,-1-1 0,0 0 0,0 0 0,-1-1 0,1 1-1,-2-1 1,1 0 0,-1 0 0,0-1 0,0 0 0,0 0 0,-1 0 0,0-1 0,1 0 0,-2 0 0,1-1 0,-3 2-25,7-5 27,0-1 0,1 1-1,-1 0 1,1-1 0,-1 1 0,0-1 0,1 0-1,-1 0 1,1 0 0,0 0 0,-1-1 0,1 1-1,0 0 1,0-1 0,0 0 0,0 1 0,0-1-1,0 0 1,0 0 0,0 0 0,1 0 0,-1-1-1,1 1 1,0 0 0,0-1 0,-1 1 0,2-1-1,-1 1 1,0-1 0,0 1 0,1-1 0,-1 1-1,1-1 1,0 0 0,0 1 0,0-1 0,0 0 0,0 1-1,1-2-26,-2-2 25,1 0 0,0 0 1,0 0-1,1 1 0,0-1 0,0 0 0,0 0 0,0 1 0,1-1 0,0 0 0,0 1 0,1 0 0,-1-1 0,1 1 0,0 0 0,1 1 0,-1-1 1,1 0-1,0 1 0,0 0-25,-2 3-9,-1 0 0,1 0 0,0 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,-1 1 0,1 0 0,0-1 0,0 1 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 1 0,0-1 0,-1 1 1,1-1-1,0 1 0,0-1 0,-1 1 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,0 0 0,1 0 0,-1 1 0,1 0 9,2 1-93,0 1 0,-1 0-1,1 0 1,-1 1 0,0-1 0,0 1 0,-1-1-1,1 1 1,-1 0 0,0 0 0,1 3 93,-2-3 3,0 1 1,0-1 0,0 1 0,-1-1-1,0 1 1,0-1 0,0 1 0,-1 0-1,1-1 1,-1 0 0,-1 1 0,1-1-1,-1 1 1,0-1 0,0 0 0,-1 0-1,1 0 1,-1-1 0,0 1 0,0 0 0,-1-1-1,1 0 1,-1 0 0,0 0 0,0 0-1,-1-1 1,-1 2-4,4-4 46,0 1-1,-1-1 1,1 0 0,-1 0-1,1 0 1,-1 0 0,0 0-1,1-1 1,-1 1 0,0-1-1,0 1 1,1-1 0,-1 0-1,0 0 1,0 0 0,1-1-1,-1 1 1,0-1 0,1 1-1,-1-1 1,0 0 0,1 0-1,-1 0 1,1 0 0,-1-1-1,1 1 1,0-1 0,0 1-1,-1-1 1,1 0 0,0 0-1,-1-2-45,-2-4 33,0 0-1,1-1 0,0 0 1,0 0-1,1 0 0,1 0 1,-1 0-1,1-1 0,1 1 1,0-1-1,0 0 1,1 1-1,0-1 0,0 1 1,2-2-33,-2 9 10,0-1 1,0 1 0,0-1-1,1 1 1,0-1 0,-1 1-1,1-1 1,0 1 0,0 0-1,0-1 1,0 1 0,1 0-1,-1 0 1,1 0 0,-1 0-1,1 0 1,0 0 0,0 0-1,-1 1 1,1-1 0,0 1-1,1-1 1,-1 1 0,0 0-1,0 0 1,2-1-11,2 2-6,1 1 1,-1 0-1,0 0 1,0 1-1,0 0 0,0 0 1,-1 0-1,1 1 0,0 0 1,-1 0-1,0 0 1,0 1-1,0-1 0,0 1 1,0 1-1,-1-1 1,3 3 5,-7-7-1,3 3 0,1-1 1,-1 1-1,0 0 0,0 0 1,0 0-1,-1 0 1,1 0-1,-1 1 0,0-1 1,0 1-1,0 0 0,0 0 1,0-1-1,-1 1 1,0 0-1,0 0 0,0 1 1,0-1-1,-1 0 0,1 0 1,-1 0-1,0 0 1,0 0-1,-1 1 0,1-1 1,-1 0-1,0 0 0,0 0 1,-1 0-1,1 0 1,-1 0-1,1-1 0,-1 1 1,-1 1 0,1-4 2,1 0 0,0 0 0,0 0 1,0 0-1,-1 0 0,1 0 0,-1-1 1,1 1-1,-1 0 0,1-1 0,-1 1 1,1-1-1,-1 0 0,1 1 0,-1-1 0,1 0 1,-1 0-1,0 0 0,1 0 0,-1 0 1,1 0-1,-1-1 0,0 1 0,1 0 1,-1-1-1,1 1 0,-1-1 0,1 0 1,0 1-1,-1-1 0,1 0 0,0 0 1,-1 0-1,1 0 0,-1-1-2,-1-1 6,0 0 0,0-1 0,0 0 0,0 1 0,0-1 0,1 0-1,0 0 1,0-1 0,0 1 0,0 0 0,1-1 0,-1-1-6,1-2 8,-1 1 0,1-1 0,1 1 0,-1-1 0,1 0 1,1 0-1,0 1 0,0-1 0,0 1 0,2-8-8,-2 13 9,0 0 0,0 0 0,-1 0 0,1-1 1,0 1-1,1 0 0,-1 0 0,0 0 0,0 1 0,1-1 0,-1 0 0,1 0 0,0 1 0,0-1 0,-1 1 1,1-1-1,0 1 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 1 0,0-1 0,1 1 1,-1-1-1,0 1 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 1 0,0-1 0,1 0 0,-1 1 1,0 0-1,1 0-9,0-1-25,1 1 1,-1 0 0,1 0 0,-1 1 0,1-1-1,-1 1 1,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 1 0,-1-1 0,1 1-1,-1 0 1,1-1 0,-1 1 0,0 0-1,0 1 1,-1-1 0,1 0 0,-1 0 0,1 1-1,-1-1 1,0 1 0,0-1 0,-1 1 0,1 0-1,-1-1 1,1 1 0,-1 0 0,0-1-1,-1 1 1,1 0 0,-1-1 0,1 1 0,-2 1 24,-1 2 21,0 1 1,-1-1 0,0 0-1,-1-1 1,1 1-1,-1-1 1,0 1 0,-1-2-1,0 1 1,0-1 0,0 1-1,0-2 1,-1 1-1,0-1 1,0 0 0,0 0-1,0-1 1,-1 1-22,5-4 24,1 1 1,0 0-1,0-1 0,0 1 1,0-1-1,-1 0 0,1 0 1,0 1-1,0-2 0,0 1 1,-1 0-1,1 0 0,0-1 1,0 1-1,0-1 0,0 0 1,0 1-1,0-1 0,0 0 1,0 0-1,0-1 0,0 1 1,0 0-1,0 0 0,1-1 1,-1 1-1,0-1 1,1 0-1,0 1 0,-1-1 1,1 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,1 0 0,-1-2-24,0-1 21,-1-1 0,1 0 0,0 1 0,1-1 0,0 0 0,-1 1 1,2-1-1,-1 0 0,1 1 0,0-1 0,0 0 0,0 1 0,1-1 0,0 1 0,0 0 0,0-1 0,1 1 0,0 0 0,0 0 0,0 1 0,1-1 0,-1 1 0,1 0 0,0-1 0,0 2 0,1-1 0,-1 0 0,1 1 0,0 0 0,-1 0 0,2 0 0,-1 1 0,0 0 0,0 0 1,1 0-1,0 0-21,-2 2-16,0-1 0,0 1 0,0 1 0,0-1 0,0 0 0,0 1 0,0 0 1,0 0-1,0 0 0,-1 0 0,1 1 0,0 0 0,-1-1 0,1 1 0,-1 1 0,1-1 1,-1 0-1,0 1 0,0 0 0,0-1 0,-1 1 0,1 0 0,0 1 0,-1-1 1,0 0-1,0 1 0,0-1 0,0 1 0,-1 0 0,1-1 0,-1 1 0,0 0 1,0 0-1,0 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,-1 0 0,1 0 1,-1 0-1,0 0 0,0 0 0,0 0 16,-1 1 21,-1-1 1,0 1-1,0-1 1,0 0-1,0 0 1,-1 0-1,1 0 1,-1 0 0,0-1-1,0 0 1,-1 0-1,1 0 1,-1 0-1,1-1 1,-3 1-22,6-2 7,-1 0 0,0 0 0,0-1 1,1 1-1,-1-1 0,0 1 1,0-1-1,0 0 0,0 0 1,1 0-1,-1 0 0,0 0 0,0 0 1,0 0-1,0-1 0,1 1 1,-1-1-1,0 1 0,0-1 1,1 0-1,-1 0 0,0 0 0,1 1 1,-1-2-1,1 1 0,-1 0 1,1 0-1,-1 0 0,1-1 1,0 1-1,0-1 0,0 1 0,0-1 1,0 1-1,0-1 0,0 0 1,0 1-1,0-1 0,1 0 1,-1 0-1,1 1 0,-1-2-7,0-2 0,-1 0 1,1 0-1,0 0 0,0 0 0,0 0 0,1 0 0,0 0 1,0 0-1,0 0 0,1 0 0,-1 1 0,1-1 0,0 0 1,1 0-1,-1 0 0,1 0 0,0 1 0,0-1 0,0 1 1,1 0-1,0-1 0,0 1 0,0 0 0,0 0 0,0 1 1,1-1-1,0 1 0,-1 0 0,1 0 0,1 0 0,-1 0 1,2 0-1,-4 3 13,0 0 1,-1 0 0,1 1 0,0-1 0,-1 0 0,1 1 0,-1 0 0,1-1-1,-1 1 1,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0-1,0 0 1,1 0 0,-1 0 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 0-1,0 1 1,0-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,-1-1-1,0 1 1,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0-1,-1-1 1,1 1 0,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 1-1,0-1 1,0 1 0,0-1 0,0 0 0,-1 1-14,2-1 11,0 0 1,0 0 0,0 0-1,0 0 1,0-1-1,-1 1 1,1 0 0,0 0-1,0-1 1,-1 1-1,1 0 1,-1 0-1,1-1 1,-1 1 0,1-1-1,-1 1 1,1 0-1,-1-1 1,1 1 0,-1-1-1,0 1 1,1-1-1,-1 1 1,0-1-1,1 0 1,-1 1 0,0-1-1,0 0 1,0 1-1,1-1 1,-1 0 0,0 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,0 0 0,0 0-1,1 0 1,-1 0-1,0-1 1,0 1 0,1 0-1,-1-1 1,0 1-1,0 0 1,1-1-1,-1 1 1,0-1 0,1 1-1,-1-1 1,0 1-1,1-1 1,-1 1 0,1-1-1,-1 0 1,1 1-1,-1-1 1,1 0-1,0 0 1,-1 1 0,1-1-1,0 0-11,-1-1-4,1-1 0,-1 1 0,1-1 0,0 1 0,0 0 0,0-1-1,0 1 1,0-1 0,1 1 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,0 0-1,1 0 1,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 1 0,0-1 0,0 0-1,0 1 1,0 0 0,0-1 0,0 1 0,0 0 0,1 0 0,-1 0 0,0 1 0,1-1-1,-1 0 1,0 1 0,1-1 0,-1 1 4,-1 1 3,0 0-1,-1 0 0,1 0 1,0 0-1,-1-1 0,1 1 1,-1 0-1,1 0 1,-1 1-1,0-1 0,1 0 1,-1 0-1,0 0 0,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,0 1-1,0-1 0,0 0 1,0 0-1,-1 0 0,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1 0 0,0-1 1,1 1-1,-1 0 1,0 0-1,0-1 0,0 1 1,0 0-1,0-1 0,1 1 1,-1-1-1,0 1 1,0-1-1,-1 1-2,0 1 9,0 0 0,0 0 0,0-1 1,-1 1-1,1-1 0,-1 1 0,1-1 1,-1 0-1,0 0 0,1 0 0,-1 0 0,0 0 1,0-1-1,0 1 0,0-1 0,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 0,0-1 1,0 1-1,0-1 0,1 0 0,-1 0 0,0 0 1,1 0-1,-1 0 0,1 0 0,-1-1 0,1 1 1,-1-1-1,1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0-1 0,1 1 1,-1-1-1,1 1 0,0-1 0,-1-1-9,-6-55-197,8 59 188,-1 0 1,1-1-1,0 1 1,1 0 0,-1 0-1,0-1 1,0 1-1,0 0 1,0-1-1,0 1 1,0 0-1,0 0 1,0-1-1,0 1 1,1 0-1,-1 0 1,0-1-1,0 1 1,0 0-1,0 0 1,1 0 0,-1-1-1,0 1 1,0 0-1,1 0 1,-1 0-1,0 0 1,0-1-1,1 1 1,-1 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,0 0 0,1 0-1,-1 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,1 0-1,-1 1 1,0-1-1,0 0 1,1 0-1,-1 0 1,0 0 0,0 0-1,0 1 1,1-1-1,-1 0 1,0 0-1,0 0 1,0 1-1,1-1 1,-1 0-1,0 0 1,0 1-1,0-1 1,0 0 8,16 17-486,-15-17 491,-1 1 1,1 0 0,0 0 0,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0-1,0 0 1,1 0 0,-1 1 0,0-1 0,0 0-1,0 0 1,0 0 0,0 0 0,-1 0 0,1 0 0,0 0-1,0 0 1,-1 1 0,1-1 0,0 0 0,-1 0-1,1 0 1,-1 0 0,0-1 0,1 1 0,-1 0 0,0 0-1,1 0 1,-1 0 0,0-1 0,0 1 0,0 0-1,0-1 1,0 1 0,0 0 0,0-1 0,0 0 0,0 1-6,0-1 8,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,1 0 0,-1-1 0,0 1 0,0-1 0,0 1 0,1-1 0,-1 0 0,0 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,0 0 0,1 0 0,0 1 0,-1-1 0,1 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0-8,3-41-91,-3 39 86,0 1 0,1-1 0,-1 1-1,1-1 1,-1 1 0,1-1 0,0 1 0,0 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,1 0-1,-1 0 1,1 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0 0 0,0 0-1,0-1 1,1 1 0,-1 0 0,1 1 0,-1-1 0,0 0 0,1 1 0,-1-1 0,1 1 0,0 0-1,-1 0 1,1 0 0,-1 0 0,1 0 0,-1 1 0,1-1 0,-1 1 0,1 0 0,-1-1 0,0 1-1,1 0 1,-1 1 0,1-1 5,-1 1-2,0 0-1,0 1 1,1-1 0,-1 0-1,-1 1 1,1 0 0,0-1-1,-1 1 1,1 0-1,-1 0 1,0 0 0,0 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,-1 1 0,0-1-1,0 0 1,0 0-1,0 0 1,0 1 0,-1-1-1,1 0 1,-1 0 0,0 0-1,0 0 1,0 0-1,0 0 1,-1 0 0,1 0-1,-1-1 1,0 1 0,0 0-1,0-1 1,0 1 2,0-3-41,1 1-1,0-1 1,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0-1,1 0 1,0 0 0,-1 0-1,1-1 1,-1 1 0,1-1-1,0 1 1,-1-1 0,1 1-1,0-1 1,0 0 0,-1 1-1,1-1 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,1 0 1,-1-1 0,0 1-1,1 0 1,-1-1 0,1 1-1,-1 0 1,1-1 0,-1 1-1,1 0 1,0-1 0,0 1-1,0-1 1,0 1 0,0-1-1,0 1 1,0 0 0,0-1-1,1 1 1,0-2 41,2-36-7232,-3 25 6294</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink29.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-06-24T04:06:41.025"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#FFFF00"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">187 196 8320,'-26'10'8447,"26"-10"-8352,-1-1-1,0 1 1,1-1-1,-1 1 1,1-1-1,-1 1 1,1-1-1,-1 0 1,1 1-1,-1-1 1,1 0-1,-1 1 1,1-1-1,0 0 1,-1 1-1,1-1 1,0 0-1,0 0 1,0 1-1,-1-1 1,1 0-1,0 0 1,0 1-1,0-1 1,0 0-1,0 0 1,1 0-1,-1 1 1,0-1-1,0 0 1,0 0-1,1 0-94,-1-3 103,1 0 0,0 0 0,0 1 0,0-1 0,0 0 0,1 0-1,-1 1 1,1-1 0,0 1 0,0-1 0,1 1 0,-1 0 0,0 0-1,1 0 1,0 0 0,0 0 0,0 1 0,0-1 0,0 1-1,0 0 1,3-1-103,-5 1-47,1 1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 1 0,0-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,-1-1 0,1 1 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 1 0,1-1 0,-1 1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 2 47,0 1-23,-2 1 0,1-1-1,0 0 1,-1 1 0,0-1 0,0 0 0,0 0-1,-1 1 1,1-1 0,-1 0 0,0 0-1,0-1 1,0 1 0,-1 0 0,1-1 0,-1 1-1,-3 2 24,5-3 54,-1-1 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0-1 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,1-1 0,-1 1 0,1-1 0,-1 0 0,1 0-54,-19-55 464,20 55-453,1 0 1,-1 0-1,1 0 1,0 1-1,0-1 0,0 0 1,0 0-1,0 0 0,0 0 1,0 1-1,1-1 1,-1 0-1,1 0 0,-1 0 1,1 1-1,0-1 1,0 0-1,0 1 0,0-1 1,0 1-1,0-1 1,0 1-1,0-1 0,0 1 1,1 0-1,-1 0 0,1 0 1,-1-1-1,1 1 1,0 0-12,-1 1-11,1-1 0,0 1 1,-1 0-1,1 0 0,0 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,-1 0 0,1 1 1,0-1-1,-1 0 0,1 1 1,0 0-1,-1-1 0,1 1 1,-1 0-1,1 0 0,-1 0 1,0 0-1,1 0 0,-1 0 1,0 0-1,0 0 0,0 1 1,1-1-1,-1 0 0,-1 1 1,1-1-1,0 1 0,0-1 1,0 1-1,-1 0 0,1-1 1,-1 1-1,1-1 0,-1 1 1,0 0-1,0 0 0,0-1 1,0 1-1,0 0 0,0-1 1,0 1-1,0 0 0,-1-1 1,1 1-1,0 0 0,-2 1 11,0 4 3,0-1 0,-1 1-1,0 0 1,0-1 0,0 0-1,-1 0 1,0 0 0,-1 0-1,1 0 1,-1-1 0,0 0-1,0 0 1,-1 0 0,1-1-1,-1 0 1,-1 1-3,5-4 11,-1 1 1,1-1-1,-1 0 0,1 0 1,-1 0-1,1 0 1,-1 0-1,0-1 0,0 1 1,1-1-1,-1 0 0,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 0,1-1 1,-1 0-1,0 1 0,1-1 1,-1 0-1,1 0 0,-1 0 1,1-1-1,0 1 1,-1-1-1,1 1 0,0-1 1,0 0-1,0 1 0,0-1 1,0 0-1,0 0 1,1-1-1,-1 1 0,1 0 1,-1-1-1,1 0-11,-2-1 23,2 0 1,-1-1-1,0 1 0,1 0 0,0-1 1,0 1-1,0-1 0,0 1 0,1-1 1,0 1-1,0-1 0,0 1 1,0-1-1,1 0 0,0 1 0,0-1 1,0 1-1,0 0 0,1-1 0,0 1 1,0 0-1,0 0 0,0 0 1,0 0-1,1 0 0,0 1 0,0-1 1,0 1-1,0 0 0,1 0 0,-1 0 1,1 0-1,1-1-23,-3 3-10,0 1 0,0-1 0,0 1 0,0 0 0,0 0 1,0 0-1,1 0 0,-1 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 1 0,0-1 0,-1 1 0,1 0 1,0 0-1,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 1 0,1-1 0,-1 1 0,1-1 1,-1 1-1,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,-1 0 0,1 0 1,0 0-1,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 1,-1 0-1,0 2 10,-1 8 12,-1 0 0,0 0 0,-1 0 1,0 0-1,-1-1 0,0 0 1,-1 0-1,0 0 0,-1 0 0,-7 8-12,14-18 9,-1 0 1,0 0-1,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 1,0 0-1,0-1 0,0 1 0,0 0 0,0 0 0,0-1 1,0 1-1,0-1 0,0 1 0,-1-1 0,1 0 0,0 1 1,0-1-1,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,-1 0 0,1-1 0,0 1 0,0-1 1,0 1-1,-1 0 0,1-1 0,0 0 0,0 1 0,0-1 1,0 0-10,-2-7 42,0 0 0,1 1 0,0-1 1,1 0-1,0 0 0,0-1 0,1 1 0,0 0 1,0 0-1,1 0 0,0 0 0,2-7-42,-2 6 51,1 1 0,0-1-1,1 0 1,0 1 0,0 0-1,0 0 1,1 0 0,1 0-1,-1 1 1,2-3-51,-4 8 8,0 0 0,-1-1 0,1 1-1,0 0 1,0 0 0,1 0 0,-1 0 0,0 1 0,1-1-1,-1 0 1,0 1 0,1 0 0,0-1 0,-1 1 0,1 0-1,0 1 1,0-1 0,0 0 0,-1 1 0,1-1-1,0 1 1,0 0 0,0 0 0,0 0 0,0 1 0,0-1-1,0 1 1,-1-1 0,1 1 0,0 0 0,0 0 0,0 1-8,1-1-31,0 1 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0 1 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 1 0,-1-1 0,0 1 0,0-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,-1 0 31,0 2 2,0 1-1,-1-1 1,1 0 0,-1 0-1,0 1 1,-1-1 0,0 0 0,0 0-1,0 0 1,-1 0 0,1 0-1,-1 0 1,-1 0 0,1-1 0,-1 1-1,0-1 1,0 1 0,-1-1-1,0 0 1,0 0 0,0-1-1,0 1 1,-1-1 0,1 0 0,-4 2-2,7-6 8,-1 1 0,1 0 0,-1-1 0,1 1 0,-1-1 0,1 0 1,-1 0-1,1 1 0,-1-1 0,1 0 0,-1 0 0,1 0 1,-1 0-1,1-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,-1-1 1,1 1-1,-1-1 0,1 0 0,0 0 0,-1 1 0,1-1 0,0 0 1,0 0-1,0 0 0,-1 0 0,1-1 0,0 1 0,0 0 0,1 0 1,-1-1-1,0 1 0,0 0 0,1-1 0,-1 1 0,0-1-8,-21-60 312,20 50-257,0 0-1,0 0 1,2 0 0,-1 0-1,1 0 1,1-1 0,0 1-1,1 0 1,1 1 0,-1-1-1,2 0 1,4-9-55,-6 18-6,1 0-1,0 1 1,-1-1 0,1 1 0,1 0-1,-1 0 1,0 0 0,0 0-1,1 1 1,-1-1 0,1 1 0,-1 0-1,1 0 1,0 0 0,-1 1 0,1-1-1,0 1 1,0 0 0,-1 0 0,1 0-1,0 0 1,0 1 0,-1-1-1,1 1 1,0 0 0,-1 0 0,1 1-1,-1-1 1,0 1 0,1 0 0,-1-1-1,0 1 1,0 1 0,0-1 0,0 0-1,0 1 1,0 0 0,-1-1-1,0 1 1,3 3 6,-3-2-33,1 0-1,-1 1 0,0-1 1,0 1-1,0 0 1,-1 0-1,0-1 0,0 1 1,0 0-1,0 0 1,-1 0-1,0 0 0,0 0 1,0 0-1,0 0 1,-1 0-1,0 0 0,0 0 1,-1 0-1,1-1 1,-1 1-1,0 0 0,-1 0 34,-1 4-6,0 0 0,-1-1-1,0 0 1,0 0 0,-1-1-1,0 1 1,-1-1 0,1 0-1,-1-1 1,-1 0 0,-5 4 6,12-9 11,-1 1 1,0-1-1,0 1 1,0-1-1,0 0 1,0 0-1,0 0 1,0 0 0,0-1-1,0 1 1,0 0-1,0-1 1,-1 0-1,1 1 1,0-1-1,0 0 1,-1 0 0,1 0-1,0 0 1,0-1-1,0 1 1,-1-1-1,1 1 1,0-1-1,0 0 1,0 1 0,0-1-1,0 0 1,0-1-1,0 1 1,0 0-1,0-1 1,1 1-1,-1 0 1,1-1 0,-1 0-1,1 1 1,-1-1-1,1 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,1-1-1,-1 0-11,0-4 26,0 1-1,1 0 0,-1-1 0,2 1 1,-1-1-1,0 1 0,1-1 0,1 1 1,-1-1-1,1 1 0,0 0 1,0 0-1,0 0 0,1 0 0,0 0 1,1 0-1,-1 1 0,1 0 0,0 0 1,0 0-1,1 0 0,-1 0 1,6-3-26,-8 7-10,0 0 0,0 0 1,-1 0-1,1 0 0,0 1 1,0-1-1,1 1 1,-1-1-1,0 1 0,0 0 1,0 0-1,0-1 0,0 2 1,0-1-1,0 0 1,0 0-1,1 1 0,-1-1 1,0 1-1,0 0 0,0-1 1,-1 1-1,1 0 1,0 0-1,0 0 0,0 1 1,-1-1-1,1 0 0,0 1 1,-1-1-1,1 1 1,-1-1-1,0 1 0,1 0 1,-1-1-1,0 1 0,0 0 1,0 0-1,0 0 0,-1 0 1,1 1 9,2 9-19,-1 0 0,-1 0 0,0 0 0,-1 1 0,0-1 0,-1 0 0,0 0 0,-1 0 0,0 0 0,-1 0 0,0 0 0,-1-1 0,-1 1 0,1-1 0,-2 0 1,0-1-1,0 1 0,-1-1 19,7-8 1,-1-1 1,1 0 0,-1 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,0 1 0,1-1-1,-1 0 1,0 0 0,0 0 0,0 0 0,-1-1 0,1 1 0,0 0 0,0 0-1,0-1 1,-1 1 0,1 0 0,0-1 0,-1 0 0,1 1 0,0-1 0,-1 0 0,1 1-1,-1-1 1,1 0 0,0 0 0,-1 0 0,1 0 0,-1-1 0,1 1 0,-2 0-2,1-4 22,0-1 1,1 1 0,-1 0-1,0-1 1,1 1 0,0-1-1,0 1 1,1-1 0,-1 1-1,1-1 1,0 0 0,0 1-1,1-1 1,-1 1 0,1-1-1,1-1-22,-1-5 79,2 0-1,-1 1 1,1-1-1,1 1 1,0 0-1,1 0 1,-1 0 0,2 1-1,0 0 1,0 0-1,6-7-78,-10 14 4,0 0-1,0-1 1,1 1-1,-1 1 1,1-1-1,-1 0 1,1 0-1,-1 1 1,1 0-1,0-1 1,0 1-1,0 0 1,0 1-1,0-1 1,0 0-1,0 1 1,0-1-1,0 1 1,0 0 0,0 0-1,0 1 1,0-1-1,0 0 1,0 1-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,-1 0-1,1 1 1,0-1-1,-1 1 1,1 0-1,-1 0 1,0 0-1,0 0 1,1 0-1,-1 1 1,-1-1-1,1 1 1,0-1-1,0 1 1,0 1-4,-1 2-9,0 1 0,0-1 0,0 1 0,-1-1 0,0 0 0,0 1 0,-1-1-1,0 1 1,0-1 0,0 0 0,-1 1 0,0-1 0,0 0 0,0 0 0,-1 0 0,0 0 0,0-1 0,-1 1 0,1-1 0,-1 0 0,0 0 0,-1 0 0,1-1 0,-1 1 0,0-1 0,0 0 0,0 0-1,-1-1 1,0 0 0,1 0 0,-1 0 0,0-1 0,-5 2 9,8-3 1,1 0-1,0-1 0,-1 0 0,1 1 1,-1-1-1,1 0 0,-1 0 0,1 0 1,0-1-1,-1 1 0,1-1 1,-1 1-1,1-1 0,0 0 0,-1 1 1,1-1-1,0-1 0,0 1 1,0 0-1,0 0 0,0-1 0,0 1 1,0-1-1,0 0 0,0 0 1,1 1-1,-1-1 0,1 0 0,-1 0 1,1 0-1,0-1 0,0 1 1,0 0-1,0 0 0,0-1 0,1 1 1,-1 0-1,1-1 0,-2-1 17,0-1-1,1 1 1,0-1 0,0 0 0,0 1 0,1-1-1,0 0 1,0 0 0,0 1 0,0-1-1,1 0 1,-1 1 0,1-1 0,0 0 0,1 1-1,-1-1 1,1 1 0,0 0 0,0 0 0,0-1-1,1 1 1,0 0 0,-1 1 0,1-1-1,1 1 1,-1-1 0,0 1 0,1 0 0,0 0-1,-1 0 1,1 0 0,0 1 0,1 0-1,-1 0 1,0 0 0,1 0 0,-1 1 0,1-1-1,-1 1 1,1 0 0,3 0-17,-6 1 7,-1 0 0,1 0 1,0 0-1,0 0 0,0 0 0,0 1 1,0-1-1,-1 1 0,1-1 0,0 1 1,0-1-1,-1 1 0,1 0 0,0 0 1,-1 0-1,1 0 0,-1 0 0,1 0 1,-1 0-1,0 1 0,1-1 0,-1 1 0,0-1 1,0 1-1,0-1 0,0 1 0,0-1 1,0 1-1,-1 0 0,1-1 0,0 1 1,-1 0-1,1 0-7,-1 3 5,1-1 0,-1 1 0,0 0 0,0 0 0,-1 0 0,1-1 0,-1 1 0,0 0 0,0-1 0,-1 1 0,1-1 0,-3 5-5,-33 39-1371,37-48 1215,0 1 1,-1-1-1,1 1 1,-1-1-1,1 0 0,-1 1 1,1-1-1,-1 0 1,1 1-1,-1-1 0,1 0 1,-1 0-1,0 1 1,1-1-1,-1 0 0,1 0 1,-1 0-1,0 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,0 0 1,1 0-1,-1 0 0,0 0 1,1-1-1,-1 1 1,1 0-1,-1 0 0,1-1 1,-1 1-1,1 0 1,-1-1-1,1 1 0,-1 0 1,1-1-1,-1 1 1,1-1-1,-1 1 156,-3-9-411</inkml:trace>
+</inkml:ink>
+</file>
+
 <file path=xl/ink/ink3.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
@@ -2112,6 +3225,90 @@
       <inkml:brushProperty name="width" value="0.05" units="cm"/>
       <inkml:brushProperty name="height" value="0.05" units="cm"/>
       <inkml:brushProperty name="color" value="#66CC00"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">175 186 8064,'0'0'2672,"0"4"2400,7-5-4745,-6 1-315,0-1 0,0 1 0,-1-1 0,1 1 0,0 0 0,0-1 0,0 1-1,0 0 1,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,0 0 0,0-1 0,-1 1 0,1 0 0,-1 0 0,1 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,-1 0-12,-1 3 172,0-1 1,0 1-1,-1-1 0,1 1 0,-1-1 1,0 0-1,0 0 0,0 0 1,-1-1-1,1 1 0,0-1 0,-1 0 1,0 0-1,0 0 0,1 0 0,-1-1 1,0 1-1,-1-1 0,1 0 0,-2 0-172,4-2 37,0 0-1,1 0 0,-1-1 0,0 1 0,1 0 0,0-1 1,-1 1-1,1-1 0,0 0 0,0 1 0,0-1 1,0 0-1,0 0 0,0 0 0,0 0 0,1 0 0,-1 1 1,1-1-1,-1-1 0,1 1 0,0 0 0,-1 0 0,1 0 1,1 0-1,-1 0 0,0 0 0,0 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,1 0-36,0 0 0,-1-4-4,1 1 1,-1-1-1,1 0 1,1 1-1,-1-1 1,1 1 0,0 0-1,1-1 1,-1 1-1,1 0 1,0 0-1,0 1 1,0-1 0,1 1-1,0-1 1,0 1-1,0 0 1,0 0-1,1 1 1,-1-1-1,1 1 1,0 0 0,0 1-1,0-1 1,0 1-1,0 0 1,1 0-1,-1 0 1,1 1-1,0 0 1,-1 0 3,-4 1-9,0 0 1,1 0-1,-1 0 0,0 0 0,0 0 1,0 1-1,0-1 0,0 0 1,0 1-1,0-1 0,0 0 0,0 1 1,0 0-1,0-1 0,0 1 1,0-1-1,-1 1 0,1 0 0,0 0 1,0 0-1,-1-1 0,1 1 0,0 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 1,1 0-1,-1 1 0,0-1 0,0 0 1,0 0-1,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,-1 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,1 0 1,-1 0-1,0 0 0,1-1 1,-1 1-1,0 0 0,0 0 0,0-1 1,0 1-1,0 0 0,0-1 0,0 1 1,0-1 8,-1 3 30,0 0 1,-1-1-1,0 1 0,1-1 1,-1 1-1,0-1 1,0 0-1,-1 0 0,1-1 1,0 1-1,-1 0 1,1-1-1,-1 0 0,1 0 1,-1 0-1,1 0 1,-1-1-1,0 1 1,1-1-1,-1 0 0,0 0 1,0 0-1,1-1 1,-1 1-1,0-1 0,1 0 1,-1 0-1,1 0 1,-1-1-1,1 1 0,0-1 1,-1 0-1,1 0 1,0 0-1,0 0 1,0 0-1,1-1 0,-1 1 1,0-1-1,1 0 1,0 0-1,-1 0 0,1 0 1,1 0-1,-1 0 1,0-1-1,1 1-30,-1 0 10,1-1 1,0 1-1,0 0 1,0-1-1,1 1 1,-1-1-1,1 1 1,0-1-1,0 1 1,0-1-1,0 1 1,1 0-1,0-1 1,-1 1-1,1-1 1,0 1-1,1 0 1,-1 0-1,0 0 1,1-1-1,0 1 1,0 1-1,0-1 1,0 0-1,0 0 1,0 1-1,1-1 1,-1 1-1,1 0 1,0 0-1,3-2-10,-5 3-15,1 1-1,0-1 1,0 1-1,-1-1 1,1 1-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0-1,0 0 1,0 0-1,-1 0 1,1 1-1,0-1 1,0 1-1,-1 0 1,1-1-1,0 1 1,-1 0-1,1 0 1,-1 0 0,1 0-1,-1 0 1,1 0-1,-1 0 1,0 1-1,0-1 1,0 1-1,1-1 1,-1 0-1,0 2 16,28 52-598,-28-48 604,1 0-1,-1 0 1,0 1-1,-1-1 1,0 0-1,0 0 1,0 0-1,-1 0 1,0 0-1,-1 0 1,1 0-1,-1 0 1,-1 0-1,1 0 1,-1-1-1,0 1 1,-1-1-1,0 0 1,0 0-1,0 0 1,0-1-1,-1 1 1,0-1-1,0 0 1,-1-1-1,1 1 1,-1-1-1,0 0 1,0 0-1,0-1 1,-6 3-6,9-6 10,1 0 1,-1 1-1,0-1 1,1 0-1,-1 0 1,0-1-1,1 1 1,-1 0-1,1-1 1,-1 0-1,0 0 1,1 1 0,-1-2-1,1 1 1,0 0-1,-1 0 1,1-1-1,0 1 1,0-1-1,0 0 1,0 1-1,0-1 1,0 0-1,0 0 1,1-1-1,-1 1 1,1 0-1,-1 0 1,1-1-1,0 1 1,0-1-1,0 1 1,0-1 0,1 1-1,-1-1 1,1 0-1,-1 1 1,1-3-11,-1 2-4,0-1 1,1 1 0,-1 0 0,1-1 0,0 1 0,0 0-1,0-1 1,0 1 0,1 0 0,-1 0 0,1-1 0,0 1-1,0 0 1,0 0 0,0 0 0,0 0 0,1 0 0,-1 0-1,1 0 1,0 0 0,0 0 0,0 1 0,0-1-1,1 1 1,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0-1,0 0 1,0 0 0,0 1 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,1 0 0,-1 1 0,0-1 0,1 1-1,2 0 4,-2 1-37,1 0 0,-1 1 0,0-1 0,0 1 0,0 0 0,1 0 0,-2 0 1,1 0-1,0 1 0,0-1 0,-1 1 0,1 0 0,-1 0 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,0 1 0,0-1 0,0 1 0,0-1 0,-1 1 0,1-1 0,-1 1 0,0-1 0,-1 1 0,1-1 0,-1 1 0,0-1 0,0 0 0,0 1 0,-1-1 0,1 0 0,-1 0 0,0 0 0,0 0 0,-1 0 0,-1 3 37,1-4 66,0 0 0,0 1 0,0-1 0,0 0 0,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 1 0,0-1 0,0 0 0,0-1 0,0 1 0,-1-1 0,1 0 0,-4 1-66,3-3 39,-1 0 1,1 0-1,0-1 0,0 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,1-1 0,-1 0 1,1 0-1,0-1 0,0 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,1-1 0,0 1 1,1-1-1,-1 0 0,1 0 0,0 1 0,0-1 0,1-1 0,-1 1 0,1 0 0,0 0 1,1 0-1,-1-1 0,1 1 0,0 0 0,0-1 0,1 1 0,-1 0 0,1 0 0,1-1 1,-1 1-1,1-1-39,-1 1-3,0 1 0,0 0 0,1 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,1 0 0,-1 1 1,1-1-1,0 1 0,0 0 0,0 0 0,0 0 1,0 0-1,1 0 0,-1 0 0,1 1 0,1-1 3,3 1-52,1 1 0,-1 0 1,1 1-1,-1 0 0,1 0 0,-1 0 0,1 1 0,-1 1 0,0-1 0,1 2 0,-1-1 0,0 1 0,0 0 0,0 0 0,-1 1 0,1 0 1,-1 1-1,0-1 0,2 3 52,-6-5-13,0-1 0,0 1 0,0-1 1,0 1-1,0 0 0,0 0 0,-1 1 1,1-1-1,-1 0 0,1 1 1,-1-1-1,0 1 0,0 0 0,0 0 1,-1 0-1,1 0 0,-1 0 0,1 0 1,-1 1-1,0-1 0,0 0 0,0 0 1,-1 1-1,1-1 0,-1 1 0,0-1 1,0 1-1,0-1 0,-1 0 0,1 1 1,-1-1-1,1 1 0,-1-1 1,0 0-1,0 0 0,-1 2 13,-5 1 16,1 0-1,-1-1 1,0 0 0,-1 0 0,1-1-1,-1 0 1,0 0 0,0 0 0,0-1-1,-1 0 1,1-1 0,-1 0 0,1 0-1,-1-1 1,0 0 0,0-1-1,1 0 1,-1 0 0,0-1 0,0 0-16,2 1 35,0 0 1,0-1-1,0 0 0,0 0 1,0 0-1,0-1 1,0 0-1,0-1 1,1 1-1,-1-1 1,-1-2-36,5 4 21,1-1 1,0 1 0,0-1 0,-1 0 0,1 0 0,0 0 0,1 0 0,-1 0-1,0-1 1,1 1 0,-1 0 0,1-1 0,-1 1 0,1-1 0,0 1-1,0-1 1,0 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 0-1,0 1 1,0-1 0,0 0 0,1 0 0,-1 0 0,1 1 0,-1-1-22,1 0 7,-1 0 0,1 0 1,0 0-1,0 0 1,0 1-1,1-1 0,-1 0 1,1 1-1,-1-1 1,1 1-1,0-1 0,0 1 1,0 0-1,0 0 1,0-1-1,1 2 0,-1-1 1,0 0-1,1 0 1,0 1-1,-1 0 0,1-1 1,0 1-1,0 0 1,0 0-1,-1 0 0,1 1 1,0-1-1,0 1 1,0 0-1,1 0-7,5 0-79,0 0 0,-1 1 0,1 1 0,0-1 0,0 1 0,-1 1 0,1 0 0,-1 0 0,0 0 0,0 1 0,0 1 0,0-1 0,-1 1 0,0 0 0,0 1 0,6 5 79,-11-7-12,0-1-1,0 0 1,-1 1 0,1-1-1,-1 1 1,1 0 0,-1-1-1,0 1 1,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0-1,0-1 1,-1 1 0,1 0-1,-1 0 1,1 0-1,-1 0 1,-1-1 0,1 1-1,0 0 1,-1-1 0,0 1-1,1-1 1,-1 0 0,-1 1-1,1-1 1,0 0 0,-1 0-1,0 0 1,1-1 0,-1 1-1,0-1 1,-3 2 12,3-3 28,1 1 1,-1-1-1,0 0 0,0 0 1,0 0-1,-1 0 0,1-1 1,0 1-1,0-1 0,0 0 1,0 0-1,0 0 0,-1 0 0,1-1 1,0 1-1,0-1 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0-1 0,1 1 1,-1-1-1,0 0 0,1 0 1,-1 0-1,1 0 0,0 0 1,0 0-1,0-1 0,0 1 1,0-1-1,0 1 0,1-1 0,-1 0 1,1 0-1,0 0 0,-1 0 1,1 0-1,1 0 0,-1-2-28,-3-3 22,1 0 0,0 0-1,0-1 1,1 1-1,0-1 1,1 0 0,0 0-1,0 0 1,1 1-1,0-1 1,1 0 0,0 0-1,0 0 1,1 1-1,0-1 1,0 0 0,1 1-1,0 0 1,1-1-1,3-5-21,-4 11-3,1 0 0,-1 0 1,0 0-1,1 0 0,-1 1 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 1,0 1-1,1 0 0,-1 1 0,0-1 0,1 1 0,-1 0 0,0 0 0,1 0 0,-1 1 0,4 0 3,1-1-37,1 0 0,-1 1-1,0 0 1,0 1 0,0 0-1,0 0 1,0 1 0,0 0-1,-1 1 1,1 0 0,-1 0-1,0 0 1,0 1 0,-1 1-1,1-1 1,-1 1 0,0 1-1,0 0 38,-6-6-1,1 1-1,-1 0 0,0 0 0,0-1 1,0 1-1,0 0 0,0 0 0,0 0 1,-1 0-1,1 0 0,-1 0 0,1 0 1,-1 0-1,0 0 0,0 0 0,0 0 1,0 1-1,0-1 0,0 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,0 0 1,0 0-1,1 0 0,-1 0 0,0 0 1,0-1-1,-1 1 0,1 0 0,0-1 1,-1 1-1,1-1 0,-2 2 2,-66 41 211,58-40-150,1-1 1,-1 0 0,0-1 0,1 0-1,-1 0 1,0-1 0,0-1-1,0 0 1,0 0 0,0-1-1,0-1 1,0 0 0,0 0 0,0-1-62,8 2 13,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,1-1 1,-1 1-1,1-1 1,-1 0 0,1 1-1,0-1 1,-1 0-1,1-1 1,0 1 0,0 0-1,0 0 1,1-1-1,-1 0 1,1 1 0,-1-1-1,1 0 1,0 1-1,0-1 1,0 0 0,0 0-1,1 0 1,-1 0-1,1 0 1,0 0 0,-1 0-1,1 0 1,1 0-1,-1 0 1,0 0 0,1 0-1,0 0 1,-1 0-1,1 0 1,0 1 0,1-2-14,1 2-3,-1-1 0,1 1 0,0 0 0,0 0 0,0 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,1 0 0,-1 0 0,0 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1 0 0,0 1 0,-1-1 0,1 0 0,-1 1 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 1 0,-1-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,2 2 3,-2-2-89,-1-1-1,1 1 1,-1-1-1,0 1 1,0 0 0,0 0-1,0-1 1,0 1-1,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,-1 0 0,0 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,-1 0 1,1 0-1,0 1 1,0-1-1,-1 0 1,0 0 0,1-1-1,-1 1 1,0 0-1,0 0 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,-1-1 1,1 1 0,-1-1-1,1 0 1,-1 1-1,0-1 1,1 0-1,-1 0 1,0 0-1,-1 1 90,-10-2-1189,-4-10 554</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink30.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-06-24T04:06:41.026"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#004F8B"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">155 102 5120,'1'-3'349,"0"0"0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 1,-1-1-1,0 1 0,0 0 0,0 0 0,0-1 0,-1 1 0,1 0 0,-1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 1 0,-1-2-349,-34 30 2715,35-26-2657,1 1 0,0 0 0,0 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,0 0 0,0 1 1,0-1-1,1 0 0,-1 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,1-1 0,0 1 0,-1-1 0,1 1 0,0 0 0,0-1 1,0 1-1,0-1 0,0 1 0,0 0 0,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,1 1 0,0-1 0,-1 1 0,1-1 0,1 1-58,-1 2 18,1 0-1,-1 1 0,0-1 0,0 0 0,0 0 0,0 1 0,-1-1 0,0 1 0,0-1 1,0 0-1,0 1 0,-1-1 0,0 0 0,0 1 0,0-1 0,0 0 0,-1 0 0,1 0 1,-1 0-1,0 0 0,0 0 0,-1 0 0,1-1 0,-1 1-17,3-3 24,-1-1 0,1 1-1,0 0 1,-1-1 0,1 1-1,0 0 1,-1-1 0,1 1 0,-1-1-1,1 1 1,-1-1 0,1 1-1,-1-1 1,1 1 0,-1-1 0,0 1-1,1-1 1,-1 0 0,0 1-1,1-1 1,-1 0 0,0 0 0,0 1-1,1-1 1,-1 0 0,0 0 0,1 0-1,-1 0 1,0 0 0,0 0-1,1 0 1,-1 0 0,0 0 0,0 0-1,1-1 1,-1 1 0,0 0-1,1 0 1,-1-1 0,0 1 0,1 0-1,-1-1 1,0 1 0,1-1-1,-1 1 1,1-1 0,-1 1 0,1-1-1,-1 1 1,1-1 0,-1 0 0,1 1-1,0-1 1,-1 1 0,1-1-1,0 0 1,-1 0 0,1 1 0,0-1-1,0 0 1,0 1 0,0-1-1,0 0 1,-1 0 0,1 1 0,1-1-1,-1 0-23,-3-12 121,0 1 0,2 0 0,-1 0 0,2-1 0,-1 1 0,2-1 0,0 1-1,0 0 1,2-6-121,-3 16 7,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 0,1 0 0,0-1 0,-1 1 0,1 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,1 1 0,-1-1 0,0 0 0,1 1 0,-1-1 0,1 1 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0-1,1 0 1,-1 0 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1 0 0,1-1 0,-1 1 0,0 0 0,1-1 0,-1 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 2-7,1-2 7,0 1 0,0 0 0,0 0 0,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,0 0 0,0 0 0,0-1 0,-1 1 0,1 1 0,-1-1 0,1 0 0,-1 0 0,0 1 0,0-1 0,-1 0 0,1 1 0,-1-1 0,1 1 0,-1-1 0,0 0 0,-1 1 0,1-1 0,0 1 0,-1-1 1,0 1-1,0-1 0,0 0 0,0 0 0,0 1 0,-1-1 0,0 0 0,1 0 0,-1 0 0,0 0-7,-49 42 268,50-44-248,0 0 1,-1 0 0,1-1 0,-1 1-1,1 0 1,-1 0 0,1-1 0,-1 1-1,1-1 1,-1 0 0,0 1 0,1-1-1,-1 0 1,0 0 0,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0 0,0-1-1,1 1 1,-1-1 0,1 1 0,-1-1-1,1 0 1,-1 1 0,1-1 0,-1 0-1,1 0 1,0 0 0,-1 0 0,1 0-1,0-1 1,0 1 0,0 0 0,0 0-1,0-1 1,0 1 0,0-1-21,-1-4 13,0 0 0,0 0 0,1 0 0,0 0 0,0-1 0,1 1 0,-1 0 0,1-1 0,1 1 0,-1 0 0,1 0 0,0-1 0,1 1 0,-1 0 1,1 0-1,1 0 0,-1 0 0,2-2-13,-1 2-6,-3 3 10,1 1 0,0-1 0,0 0 0,0 1 0,0-1-1,0 1 1,1 0 0,-1-1 0,1 1 0,-1 0 0,1 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 1-1,1-1 1,-1 1 0,1-1 0,-1 1 0,1 0 0,-1 0-1,1 0 1,1 0-4,-1 3 13,-1 0-1,1 1 0,0-1 1,-1 0-1,0 1 0,1-1 1,-1 1-1,0 0 0,-1 0 1,1 0-1,0 0 0,-1 0 1,1 0-1,-1 0 0,0 0 1,0 1-1,-1-1 0,1 0 1,0 1-1,-1-1 0,0 1-12,0-3 3,2 10-6,0 1 0,-1-1 0,-1 0 0,0 1 0,-1-1 0,0 1 1,0-1-1,-1 0 0,-1 0 0,0 0 0,0 0 0,-1 0 0,-4 7 3,8-17 8,0-1-1,-1 1 1,1-1 0,0 1-1,0 0 1,0-1-1,0 1 1,-1-1 0,1 1-1,0-1 1,-1 1-1,1-1 1,0 1-1,-1-1 1,1 1 0,-1-1-1,1 1 1,0-1-1,-1 0 1,1 1 0,-1-1-1,0 0 1,1 1-1,-1-1 1,1 0 0,-1 0-1,1 1 1,-1-1-1,1 0 1,-1 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,1 0-1,-1 0 1,1 0 0,-1 0-1,0 0 1,1 0-1,-1-1 1,1 1-1,-1 0 1,1 0 0,-1-1-8,-4-6 6,2 0 0,-1-1 0,1 0 0,0 1-1,1-1 1,-1 0 0,2 0 0,-1 0 0,1-1 0,0 1 0,1-1-6,-2-7-7,1-68-81,2 82 76,-1 0 1,1 0 0,-1-1 0,1 1 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0-1,1 0 1,-1 0 0,1 0 0,-1 1-1,1-1 1,0 1 0,-1-1 0,1 1 0,0-1-1,0 1 1,0 0 0,0 0 0,0 0 0,1 0-1,-1 0 1,0 1 0,0-1 0,0 1-1,1-1 1,-1 1 0,0 0 0,1 0 0,1 0 11,2 0 24,1 1 0,0 0 0,-1 0 0,1 0 0,0 1 0,-1 0 0,0 0 1,1 1-1,-1-1 0,0 1 0,0 1 0,2 1-24,-6-4 9,0 1 0,0-1 1,0 1-1,0-1 0,0 1 0,-1 0 0,1 0 1,0 0-1,-1 0 0,0 0 0,1 0 1,-1 0-1,0 0 0,0 1 0,0-1 0,0 0 1,-1 1-1,1-1 0,-1 0 0,1 1 0,-1-1 1,0 1-1,0-1 0,0 1 0,0-1 1,0 1-1,-1-1 0,1 0 0,-1 1 0,0-1 1,0 1-1,1-1 0,-1 0 0,-1 1-9,-2 4 7,0 1 0,-1-1 1,1 0-1,-2 0 0,1-1 0,-1 1 0,0-1 0,0 0 0,-3 1-7,7-6 2,0 1 0,0 0 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,-1 0 0,1 0 0,0-1 0,-1 1 0,1 0-1,-1-1 1,1 0 0,0 1 0,-1-1 0,1 0 0,-1 0 0,1-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,0-1 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0-1,0-1 1,0 1 0,0-1 0,-1 0-2,-1-4 0,0 1 0,0-1 0,1-1 0,0 1 0,0-1 0,0 1 0,0-1 0,1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,1 0 0,0 0 0,1 0 0,-1-1 0,1 1 0,1 0 0,-1 0 0,1 0 0,0 1 0,2-5 0,-3 9 5,0 0 0,0 0-1,0 0 1,0 0 0,1 0-1,-1 0 1,0 0 0,1 1 0,-1-1-1,1 0 1,0 1 0,-1-1-1,1 1 1,0 0 0,0 0 0,0 0-1,0-1 1,0 2 0,0-1-1,0 0 1,0 0 0,1 1-1,-1-1 1,0 1 0,0 0 0,1-1-1,-1 1 1,0 0 0,0 1-1,1-1 1,-1 0 0,0 1 0,0-1-1,3 1-4,0 2 9,1 0 0,-1 1 0,1-1 0,-1 1-1,0 0 1,-1 1 0,1-1 0,-1 1 0,0 0 0,0 0-1,0 0 1,0 0 0,-1 1 0,0-1 0,0 1 0,-1 0-1,0 0 1,0 0 0,0 0 0,-1 0 0,1 1 0,-1-1-1,-1 0 1,0 1 0,1-1 0,-2 1 0,1-1 0,-1 0-1,0 1 1,0-1 0,-1 0 0,-2 6-9,2-7 6,-1 0 0,1 0 0,-1-1 1,0 1-1,-1-1 0,1 1 0,-1-1 0,0 0 1,0-1-1,0 1 0,0-1 0,-1 0 0,1 0 1,-1 0-1,0 0 0,0-1 0,0 0 0,0 0 1,0 0-1,0-1 0,-1 1 0,1-1 0,0-1 1,-1 1-1,1-1 0,-1 0 0,1 0 0,-1 0 1,1-1-1,-1 0 0,-1-1-6,2-1-4,1-1 0,0 0 0,1-1 0,-1 1 0,1-1 0,0 0 0,0 0 0,0 0 0,1 0 0,0 0 0,0 0 0,0-1 0,0 1 0,1-1 0,0 1 0,0-1 0,1 0 0,0 1 0,0-1 0,0 0 0,0 1 0,1-1 0,0 0 0,0 1 0,0-1 0,1 1 0,0-1 0,2-2 4,-4 4 1,1 0 0,0 0 0,0 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,1 1 1,0 0-1,0-1 0,0 1 0,0 0 0,1 0 0,-1 1 0,1-1 0,0 0 0,0 1 0,0-1 0,0 1 0,0 0 0,0 0 0,1 1 0,-1-1 1,1 0-1,-1 1 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 1 0,0 0 0,0-1 0,-1 1 0,1 1 0,2-1-1,-1 3 9,0 0 0,0 1 0,0-1 0,0 1 0,0 0 1,-1 0-1,0 1 0,0-1 0,0 1 0,0 0 0,-1 0 0,0 0 0,0 0 0,0 1 0,0 0 0,-1-1 0,0 1 0,0 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 1,-1 0-1,-1 0 0,1 0 0,-1 1 0,-1-1 0,1 0 0,-1-1 0,0 1 0,0 0-9,1-4 4,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0-1 1,-1 1 0,1 0-1,-1-1 1,1 0-1,-1 1 1,0-1-1,0 0 1,0 0-1,1 1 1,-1-1-1,0-1 1,0 1-1,0 0 1,0 0-1,-1-1 1,1 1-1,0-1 1,0 0-1,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,0-1 1,0 1-1,0-1 1,0 1-1,0-1 1,0 0-1,0 0 1,-2-1-5,1-4-9,-1 0 0,1 1 0,0-1 0,1-1 0,-1 1 1,1 0-1,1-1 0,-1 1 0,1-1 0,0 1 0,1-1 0,-1 0 0,1 1 0,1-1 1,-1 0 8,0 2-5,-1 0 0,1 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,0 1 0,0-1 0,1 0 0,0 1 0,0-1 0,0 1 0,0-1 1,1 1-1,-1 0 0,1 0 0,0 0 0,1 0 0,-1 1 0,1-1 0,-1 1 0,1 0 0,0 0 0,0 0 0,0 1 0,4-2 5,-6 4 3,1 1 0,0-1 0,-1 1 0,1 0 0,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,0 0-1,0 0 1,-1 0 0,1 0 0,0 0 0,-1 0 0,1 1 0,-1-1 0,0 0 0,0 1-1,0-1 1,0 1 0,0 0 0,0-1 0,-1 1 0,1-1 0,-1 1 0,0 0-1,0 0 1,0-1 0,0 1 0,0 0 0,0-1 0,-1 2-3,1 1 72,-1-1 1,0 1-1,1 0 1,-2-1-1,1 1 0,0-1 1,-1 0-1,0 1 1,0-1-1,0 0 0,-1 0 1,1 0-1,-1-1 1,0 1-1,0 0 0,0-1 1,-1 0-1,1 0 1,-1 0-1,0 0 0,1-1 1,-1 1-1,-1-1 1,1 0-1,0 0 1,-2 0-73,4-2 0,0 1 1,0-1-1,-1-1 1,1 1 0,0 0-1,0 0 1,0-1 0,0 0-1,0 1 1,0-1 0,0 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0-1 1,1 1 0,-1-1-1,0 1 1,1-1 0,0 0-1,-1 1 1,1-1-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,1 0 0,-13-26-2958,16 0-6876,9 19 8586</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink31.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-06-24T04:06:41.027"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#843C0C"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">72 202 7296,'0'0'192,"0"0"0,0-1 1,0 1-1,0 0 0,0 0 1,0 0-1,0 0 0,0-1 1,0 1-1,0 0 0,0 0 1,0 0-1,0-1 0,0 1 1,0 0-1,0 0 0,0 0 1,0-1-1,0 1 0,0 0 1,0 0-1,0 0 0,0-1 1,0 1-1,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 1,0-1-1,0 1 0,0 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,0 0 0,0 0 1,-1-1-1,1 1 0,0 0 1,0 0-1,0 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 1,0 1-1,0-1-192,9-8 588,-7 9-547,-1-1 0,1 0 0,-1 0 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 0,0 0 0,1-1 0,-1 1 0,0 0-1,0 0 1,0 0 0,0 0 0,1 0 0,-1 0 0,-1 0 0,1 0 0,0 1 0,0-1 0,0 0 0,-1 1 0,1-1 0,0 0 0,-1 1-1,0-1 1,1 0 0,-1 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 1 0,-1-1-1,1 0 1,-1 1 0,0 0-41,-13-20 720,11 9-704,1 0 0,1 0 0,-1-1 0,1 1 0,1 0 0,0 0 0,0-1 0,1 1 0,0 0 0,0 0 0,1 0 0,1 0 0,-1 0 0,1 0 0,1 1 0,0-1 0,0 1 0,1 0 0,1-2-16,-4 7 0,0 0 0,0 0 0,0 1 0,1-1 0,0 1 0,-1-1 0,1 1 0,0 0 0,0 0 0,0 0 0,0 0 0,1 1 0,-1-1 0,0 1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 1 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 1 0,0-1 0,0 1 0,1 0 0,-1 0 0,0 0 0,-1 0 0,1 1 0,0-1 0,-1 1 0,1 0 0,-1-1 0,0 1 0,0 0 0,0 1 0,1 1 0,-2 2 27,0 0 0,0 0 0,-1 0 0,0 0 0,0 0-1,0 0 1,-1 0 0,0 0 0,-1 0 0,1-1 0,-1 1-1,0 0 1,-1-1 0,0 1 0,0-1 0,0 0 0,-1 0-1,0 0 1,0 0 0,-1-1 0,1 0 0,-1 0 0,0 0-1,-1 0 1,1-1 0,-1 0 0,0 0 0,0 0 0,0-1-1,0 0 1,-2 0-27,7-2 25,0 0-1,-1 0 1,1 0-1,-1-1 0,1 1 1,-1 0-1,1-1 1,-1 1-1,1-1 0,-1 0 1,1 0-1,-1 1 1,1-1-1,-1 0 0,0 0 1,1 0-1,-1-1 0,1 1 1,-1 0-1,1-1 1,-1 1-1,1-1 0,-1 1 1,1-1-1,-1 0 1,1 1-1,-1-1 0,1 0 1,0 0-1,0 0 1,0 0-1,-1 0 0,1 0 1,0-1-1,0 1 1,0 0-1,0 0 0,1-1 1,-1 1-1,0-1-24,1-1 19,-1 0-1,1 0 0,-1 0 1,1-1-1,0 1 0,1 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,0 0 0,0 0 1,0 0-1,0 0 0,1 0 1,-1 0-19,37-35 76,-37 37-75,0 0-1,0 0 0,0 1 0,0-1 0,0 0 1,0 0-1,0 1 0,0-1 0,0 1 0,1-1 1,-1 1-1,0 0 0,0-1 0,0 1 1,1 0-1,-1 0 0,0 0 0,1 0 0,-1 0 1,0 0-1,0 0 0,1 0 0,-1 0 0,0 1 1,0-1-1,0 0 0,1 1 0,-1-1 0,0 1 1,0 0-1,0-1 0,0 1 0,0 0 0,0 0 1,0-1-1,0 1 0,0 0 0,0 0 1,-1 0-1,1 0 0,0 1 0,1 4 15,0 0 0,0 1 0,-1-1 1,0 0-1,0 1 0,-1-1 0,1 1 0,-2-1 0,1 1 0,-1-1 1,0 1-1,0-1 0,0 1 0,-1-1 0,0 0 0,0 0 0,-1 0 1,0 0-1,0 0 0,0 0 0,-1-1 0,0 0 0,0 0 0,0 0 1,-4 3-16,7-6 14,0-1 0,0 1 0,0-1 0,0 1 1,0-1-1,0 0 0,0 0 0,-1 1 0,1-1 0,0 0 1,-1 0-1,1 0 0,-1 0 0,1-1 0,-1 1 1,0 0-1,1-1 0,-1 1 0,0-1 0,0 1 0,1-1 1,-1 0-1,0 0 0,0 0 0,1 0 0,-1 0 1,0 0-1,0 0 0,1-1 0,-1 1 0,0-1 0,1 1 1,-1-1-1,0 0 0,1 1 0,-1-1 0,1 0 1,-1 0-1,1 0 0,0 0 0,-1 0 0,1-1 0,0 1 1,0 0-1,-1 0 0,1-1 0,0 0-14,-5-11 34,2 1-1,0-1 0,0 1 1,1-1-1,1 0 0,0 0 1,0-1-1,2 1 0,-1 0 1,2 0-1,0 0 0,0-1 1,2-2-34,-2 1 57,-1 14-54,0-1 0,0 0 0,0 1 0,0-1 1,0 0-1,0 1 0,0-1 0,1 0 0,-1 1 0,0-1 0,1 1 1,0-1-1,-1 0 0,1 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1 1,0 0-1,0 0 0,0-1 0,0 1 0,1 0 0,-1 0 0,0 0 1,1 0-1,-1 1 0,1-1 0,-1 0 0,1 1 0,0-1 0,-1 0 1,1 1-1,-1 0 0,1-1 0,0 1 0,-1 0 0,1 0 0,0 0 0,-1 0 1,1 0-1,0 1 0,-1-1 0,1 0 0,0 1 0,-1-1 0,1 1 1,-1 0-1,1-1 0,0 1-3,1 1 3,0 0 1,0 0-1,0 0 1,-1 1-1,1-1 1,-1 1-1,1-1 1,-1 1-1,0 0 1,0 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,-1 0-1,1 1 1,-1-1-1,-1 0 1,1 1-1,0-1 1,-1 1-1,1-1 1,-1 1-1,0-1 1,0 1-1,-1 0 1,1-1-1,-1 1 1,0-1-1,1 0 1,-2 1-4,0 4 25,0 0 1,-1-1 0,0 1-1,-1-1 1,0 0 0,0 0-1,0 0 1,-1 0 0,0-1-1,0 1 1,-1-1 0,1-1 0,-2 2-26,-51 16 273,57-22-265,-1-1-1,0 0 1,1 0 0,-1 0 0,0 0 0,1 0-1,-1 0 1,0-1 0,1 1 0,-1 0 0,1-1 0,-1 1-1,0-1 1,1 0 0,-1 1 0,1-1 0,-1 0-1,1 0 1,0 0 0,-1 0 0,1 0 0,0 0-1,0-1 1,0 1 0,0 0 0,0-1 0,0 1-1,0 0 1,0-1 0,0 1 0,1-1 0,-1 0-1,1 1 1,-1-2-8,0-1 0,0 1 0,0-1 0,0 1 0,1-1 0,0 0 0,-1 1 0,1-1 0,1 0 0,-1 1 0,0-1 0,1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,1 1 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 1 0,-1-1 0,1 1 0,0 0 0,0-1 0,0 2 0,0-1 0,3-1 0,-4 3 5,-1 0 0,0 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 1,-1 0-1,1 0 0,0 1 0,-1-1 0,1 0 0,-1 0 0,1 0 0,-1 1 0,0-1 0,1 0 0,-1 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,-1-1 0,1 0 0,0 0 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0-5,-1 1 5,-11 12 91,13-14-95,0 0 0,0 1-1,-1-1 1,1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,0 0-1,-1 0 1,1 0 0,0 0 0,0 0 0,-1 0 0,1-1 0,0 1-1,0 0 1,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0-1,0-1 1,0 1 0,0 0 0,-1 0 0,1 0 0,0 0 0,0-1-1,0 1 1,0 0 0,0 0 0,0 0 0,-1-1 0,1 1 0,0 0-1,0 0 1,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0-1-1,0 1 1,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0-1,0 0 1,0-1 0,0 1 0,0 0 0,1 0 0,-1-1 0,0 1 0,0 0-1,0 0 1,0 0-1,0-2-1,0-4-1,-1 0 0,1 0 0,1 0-1,-1 0 1,1 0 0,0 0 0,0 0-1,1 0 1,0 0 0,0 0 0,0 1 0,1-1-1,-1 1 1,1-1 2,-2 6 0,-1 0 0,0-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,0 0 0,1 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1 1 0,1-1 0,-1 0 0,0 1 0,1-1 0,-1 0 0,0 1 0,1-1 0,-1 0 0,0 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 1 0,0 0 0,8 26 0,-8-22 6,0-1 1,1 1-1,-2 0 0,1-1 1,0 1-1,-1 0 0,0-1 1,0 1-1,0-1 0,-1 1 0,0-1 1,1 1-1,-1-1 0,-1 0 1,1 0-1,-1 0 0,1 0 1,-1-1-1,-1 1 0,1-1 1,0 0-1,-2 2-6,4-5 1,1 0 0,0 1 0,0-1 0,-1 0 0,1 0 0,0 1 0,-1-1 0,1 0 0,0 0-1,0 0 1,-1 0 0,1 0 0,0 1 0,-1-1 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1-1 0,1 1 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1 0 0,0 0 0,0-1 0,-1 1 0,1 0 0,0 0-1,0-1 1,0 1 0,-1 0 0,1-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,-1-1 0,1 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,1 0 0,-1-1 0,0 1 0,0-1-1,3-23-66,-3 17 68,1 0 1,0 0 0,1 0-1,0 0 1,0 1 0,0-1-1,1 1 1,0-1 0,0 1-1,1 0 1,0 0-1,0 0 1,0 1 0,1 0-1,-1-1 1,2 0-3,-5 6 0,-1 0-1,0 0 0,0-1 1,0 1-1,0 0 1,0 0-1,0-1 1,1 1-1,-1 0 0,0 0 1,0-1-1,0 1 1,1 0-1,-1 0 1,0 0-1,0 0 0,1-1 1,-1 1-1,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 0,0 0 1,1 0-1,-1 0 1,0 0-1,1 0 1,-1 0-1,0 0 0,1 0 1,-1 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 0,0 0 1,1 0-1,-1 0 1,0 1-1,0-1 1,1 0-1,-1 0 1,0 0-1,0 0 0,1 1 1,-1-1-1,0 0 1,0 0-1,0 1 1,0-1-1,1 0 0,-1 0 1,0 1-1,0-1 1,0 0-1,0 0 1,0 1-1,0-1 0,0 0 1,0 0-1,0 1 1,0-1 0,-9 18 79,8-17-104,0 0 1,1-1-1,-1 1 1,0 0-1,0 0 0,0 0 1,0-1-1,0 1 1,0 0-1,0-1 1,-1 1-1,1-1 0,0 1 1,0-1-1,0 0 1,0 1-1,-1-1 1,1 0-1,0 0 0,0 0 1,-1 0-1,1 0 1,0 0-1,0 0 1,0-1-1,-1 1 0,1 0 1,0-1 24,1 1-551,1-1-1,0 0 1,-1 0 0,1 0-1,0 0 1,0 1 0,-1-1 0,1 0-1,0 1 1,0-1 0,0 1-1,0-1 1,0 1 0,0-1 0,0 1-1,0-1 1,0 1 0,0 0-1,0 0 1,0 0 0,0-1 0,0 1-1,0 0 1,0 0 0,0 0-1,1 1 1,-1-1 0,0 0 0,0 0-1,0 1 1,0-1 551,9 0-1859,8-3 126</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink32.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-06-24T04:06:41.028"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#385723"/>
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">175 186 8064,'0'0'2672,"0"4"2400,7-5-4745,-6 1-315,0-1 0,0 1 0,-1-1 0,1 1 0,0 0 0,0-1 0,0 1-1,0 0 1,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,0 0 0,0-1 0,-1 1 0,1 0 0,-1 0 0,1 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,-1 0-12,-1 3 172,0-1 1,0 1-1,-1-1 0,1 1 0,-1-1 1,0 0-1,0 0 0,0 0 1,-1-1-1,1 1 0,0-1 0,-1 0 1,0 0-1,0 0 0,1 0 0,-1-1 1,0 1-1,-1-1 0,1 0 0,-2 0-172,4-2 37,0 0-1,1 0 0,-1-1 0,0 1 0,1 0 0,0-1 1,-1 1-1,1-1 0,0 0 0,0 1 0,0-1 1,0 0-1,0 0 0,0 0 0,0 0 0,1 0 0,-1 1 1,1-1-1,-1-1 0,1 1 0,0 0 0,-1 0 0,1 0 1,1 0-1,-1 0 0,0 0 0,0 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,1 0-36,0 0 0,-1-4-4,1 1 1,-1-1-1,1 0 1,1 1-1,-1-1 1,1 1 0,0 0-1,1-1 1,-1 1-1,1 0 1,0 0-1,0 1 1,0-1 0,1 1-1,0-1 1,0 1-1,0 0 1,0 0-1,1 1 1,-1-1-1,1 1 1,0 0 0,0 1-1,0-1 1,0 1-1,0 0 1,1 0-1,-1 0 1,1 1-1,0 0 1,-1 0 3,-4 1-9,0 0 1,1 0-1,-1 0 0,0 0 0,0 0 1,0 1-1,0-1 0,0 0 1,0 1-1,0-1 0,0 0 0,0 1 1,0 0-1,0-1 0,0 1 1,0-1-1,-1 1 0,1 0 0,0 0 1,0 0-1,-1-1 0,1 1 0,0 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 1,1 0-1,-1 1 0,0-1 0,0 0 1,0 0-1,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,-1 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,1 0 1,-1 0-1,0 0 0,1-1 1,-1 1-1,0 0 0,0 0 0,0-1 1,0 1-1,0 0 0,0-1 0,0 1 1,0-1 8,-1 3 30,0 0 1,-1-1-1,0 1 0,1-1 1,-1 1-1,0-1 1,0 0-1,-1 0 0,1-1 1,0 1-1,-1 0 1,1-1-1,-1 0 0,1 0 1,-1 0-1,1 0 1,-1-1-1,0 1 1,1-1-1,-1 0 0,0 0 1,0 0-1,1-1 1,-1 1-1,0-1 0,1 0 1,-1 0-1,1 0 1,-1-1-1,1 1 0,0-1 1,-1 0-1,1 0 1,0 0-1,0 0 1,0 0-1,1-1 0,-1 1 1,0-1-1,1 0 1,0 0-1,-1 0 0,1 0 1,1 0-1,-1 0 1,0-1-1,1 1-30,-1 0 10,1-1 1,0 1-1,0 0 1,0-1-1,1 1 1,-1-1-1,1 1 1,0-1-1,0 1 1,0-1-1,0 1 1,1 0-1,0-1 1,-1 1-1,1-1 1,0 1-1,1 0 1,-1 0-1,0 0 1,1-1-1,0 1 1,0 1-1,0-1 1,0 0-1,0 0 1,0 1-1,1-1 1,-1 1-1,1 0 1,0 0-1,3-2-10,-5 3-15,1 1-1,0-1 1,0 1-1,-1-1 1,1 1-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0-1,0 0 1,0 0-1,-1 0 1,1 1-1,0-1 1,0 1-1,-1 0 1,1-1-1,0 1 1,-1 0-1,1 0 1,-1 0 0,1 0-1,-1 0 1,1 0-1,-1 0 1,0 1-1,0-1 1,0 1-1,1-1 1,-1 0-1,0 2 16,28 52-598,-28-48 604,1 0-1,-1 0 1,0 1-1,-1-1 1,0 0-1,0 0 1,0 0-1,-1 0 1,0 0-1,-1 0 1,1 0-1,-1 0 1,-1 0-1,1 0 1,-1-1-1,0 1 1,-1-1-1,0 0 1,0 0-1,0 0 1,0-1-1,-1 1 1,0-1-1,0 0 1,-1-1-1,1 1 1,-1-1-1,0 0 1,0 0-1,0-1 1,-6 3-6,9-6 10,1 0 1,-1 1-1,0-1 1,1 0-1,-1 0 1,0-1-1,1 1 1,-1 0-1,1-1 1,-1 0-1,0 0 1,1 1 0,-1-2-1,1 1 1,0 0-1,-1 0 1,1-1-1,0 1 1,0-1-1,0 0 1,0 1-1,0-1 1,0 0-1,0 0 1,1-1-1,-1 1 1,1 0-1,-1 0 1,1-1-1,0 1 1,0-1-1,0 1 1,0-1 0,1 1-1,-1-1 1,1 0-1,-1 1 1,1-3-11,-1 2-4,0-1 1,1 1 0,-1 0 0,1-1 0,0 1 0,0 0-1,0-1 1,0 1 0,1 0 0,-1 0 0,1-1 0,0 1-1,0 0 1,0 0 0,0 0 0,0 0 0,1 0 0,-1 0-1,1 0 1,0 0 0,0 0 0,0 1 0,0-1-1,1 1 1,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0-1,0 0 1,0 0 0,0 1 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,1 0 0,-1 1 0,0-1 0,1 1-1,2 0 4,-2 1-37,1 0 0,-1 1 0,0-1 0,0 1 0,0 0 0,1 0 0,-2 0 1,1 0-1,0 1 0,0-1 0,-1 1 0,1 0 0,-1 0 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,0 1 0,0-1 0,0 1 0,0-1 0,-1 1 0,1-1 0,-1 1 0,0-1 0,-1 1 0,1-1 0,-1 1 0,0-1 0,0 0 0,0 1 0,-1-1 0,1 0 0,-1 0 0,0 0 0,0 0 0,-1 0 0,-1 3 37,1-4 66,0 0 0,0 1 0,0-1 0,0 0 0,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 1 0,0-1 0,0 0 0,0-1 0,0 1 0,-1-1 0,1 0 0,-4 1-66,3-3 39,-1 0 1,1 0-1,0-1 0,0 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,1-1 0,-1 0 1,1 0-1,0-1 0,0 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,1-1 0,0 1 1,1-1-1,-1 0 0,1 0 0,0 1 0,0-1 0,1-1 0,-1 1 0,1 0 0,0 0 1,1 0-1,-1-1 0,1 1 0,0 0 0,0-1 0,1 1 0,-1 0 0,1 0 0,1-1 1,-1 1-1,1-1-39,-1 1-3,0 1 0,0 0 0,1 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,1 0 0,-1 1 1,1-1-1,0 1 0,0 0 0,0 0 0,0 0 1,0 0-1,1 0 0,-1 0 0,1 1 0,1-1 3,3 1-52,1 1 0,-1 0 1,1 1-1,-1 0 0,1 0 0,-1 0 0,1 1 0,-1 1 0,0-1 0,1 2 0,-1-1 0,0 1 0,0 0 0,0 0 0,-1 1 0,1 0 1,-1 1-1,0-1 0,2 3 52,-6-5-13,0-1 0,0 1 0,0-1 1,0 1-1,0 0 0,0 0 0,-1 1 1,1-1-1,-1 0 0,1 1 1,-1-1-1,0 1 0,0 0 0,0 0 1,-1 0-1,1 0 0,-1 0 0,1 0 1,-1 1-1,0-1 0,0 0 0,0 0 1,-1 1-1,1-1 0,-1 1 0,0-1 1,0 1-1,0-1 0,-1 0 0,1 1 1,-1-1-1,1 1 0,-1-1 1,0 0-1,0 0 0,-1 2 13,-5 1 16,1 0-1,-1-1 1,0 0 0,-1 0 0,1-1-1,-1 0 1,0 0 0,0 0 0,0-1-1,-1 0 1,1-1 0,-1 0 0,1 0-1,-1-1 1,0 0 0,0-1-1,1 0 1,-1 0 0,0-1 0,0 0-16,2 1 35,0 0 1,0-1-1,0 0 0,0 0 1,0 0-1,0-1 1,0 0-1,0-1 1,1 1-1,-1-1 1,-1-2-36,5 4 21,1-1 1,0 1 0,0-1 0,-1 0 0,1 0 0,0 0 0,1 0 0,-1 0-1,0-1 1,1 1 0,-1 0 0,1-1 0,-1 1 0,1-1 0,0 1-1,0-1 1,0 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 0-1,0 1 1,0-1 0,0 0 0,1 0 0,-1 0 0,1 1 0,-1-1-22,1 0 7,-1 0 0,1 0 1,0 0-1,0 0 1,0 1-1,1-1 0,-1 0 1,1 1-1,-1-1 1,1 1-1,0-1 0,0 1 1,0 0-1,0 0 1,0-1-1,1 2 0,-1-1 1,0 0-1,1 0 1,0 1-1,-1 0 0,1-1 1,0 1-1,0 0 1,0 0-1,-1 0 0,1 1 1,0-1-1,0 1 1,0 0-1,1 0-7,5 0-79,0 0 0,-1 1 0,1 1 0,0-1 0,0 1 0,-1 1 0,1 0 0,-1 0 0,0 0 0,0 1 0,0 1 0,0-1 0,-1 1 0,0 0 0,0 1 0,6 5 79,-11-7-12,0-1-1,0 0 1,-1 1 0,1-1-1,-1 1 1,1 0 0,-1-1-1,0 1 1,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0-1,0-1 1,-1 1 0,1 0-1,-1 0 1,1 0-1,-1 0 1,-1-1 0,1 1-1,0 0 1,-1-1 0,0 1-1,1-1 1,-1 0 0,-1 1-1,1-1 1,0 0 0,-1 0-1,0 0 1,1-1 0,-1 1-1,0-1 1,-3 2 12,3-3 28,1 1 1,-1-1-1,0 0 0,0 0 1,0 0-1,-1 0 0,1-1 1,0 1-1,0-1 0,0 0 1,0 0-1,0 0 0,-1 0 0,1-1 1,0 1-1,0-1 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0-1 0,1 1 1,-1-1-1,0 0 0,1 0 1,-1 0-1,1 0 0,0 0 1,0 0-1,0-1 0,0 1 1,0-1-1,0 1 0,1-1 0,-1 0 1,1 0-1,0 0 0,-1 0 1,1 0-1,1 0 0,-1-2-28,-3-3 22,1 0 0,0 0-1,0-1 1,1 1-1,0-1 1,1 0 0,0 0-1,0 0 1,1 1-1,0-1 1,1 0 0,0 0-1,0 0 1,1 1-1,0-1 1,0 0 0,1 1-1,0 0 1,1-1-1,3-5-21,-4 11-3,1 0 0,-1 0 1,0 0-1,1 0 0,-1 1 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 1,0 1-1,1 0 0,-1 1 0,0-1 0,1 1 0,-1 0 0,0 0 0,1 0 0,-1 1 0,4 0 3,1-1-37,1 0 0,-1 1-1,0 0 1,0 1 0,0 0-1,0 0 1,0 1 0,0 0-1,-1 1 1,1 0 0,-1 0-1,0 0 1,0 1 0,-1 1-1,1-1 1,-1 1 0,0 1-1,0 0 38,-6-6-1,1 1-1,-1 0 0,0 0 0,0-1 1,0 1-1,0 0 0,0 0 0,0 0 1,-1 0-1,1 0 0,-1 0 0,1 0 1,-1 0-1,0 0 0,0 0 0,0 0 1,0 1-1,0-1 0,0 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,0 0 1,0 0-1,1 0 0,-1 0 0,0 0 1,0-1-1,-1 1 0,1 0 0,0-1 1,-1 1-1,1-1 0,-2 2 2,-66 41 211,58-40-150,1-1 1,-1 0 0,0-1 0,1 0-1,-1 0 1,0-1 0,0-1-1,0 0 1,0 0 0,0-1-1,0-1 1,0 0 0,0 0 0,0-1-62,8 2 13,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,1-1 1,-1 1-1,1-1 1,-1 0 0,1 1-1,0-1 1,-1 0-1,1-1 1,0 1 0,0 0-1,0 0 1,1-1-1,-1 0 1,1 1 0,-1-1-1,1 0 1,0 1-1,0-1 1,0 0 0,0 0-1,1 0 1,-1 0-1,1 0 1,0 0 0,-1 0-1,1 0 1,1 0-1,-1 0 1,0 0 0,1 0-1,0 0 1,-1 0-1,1 0 1,0 1 0,1-2-14,1 2-3,-1-1 0,1 1 0,0 0 0,0 0 0,0 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,1 0 0,-1 0 0,0 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1 0 0,0 1 0,-1-1 0,1 0 0,-1 1 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 1 0,-1-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,2 2 3,-2-2-89,-1-1-1,1 1 1,-1-1-1,0 1 1,0 0 0,0 0-1,0-1 1,0 1-1,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,-1 0 0,0 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,-1 0 1,1 0-1,0 1 1,0-1-1,-1 0 1,0 0 0,1-1-1,-1 1 1,0 0-1,0 0 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,-1-1 1,1 1 0,-1-1-1,1 0 1,-1 1-1,0-1 1,1 0-1,-1 0 1,0 0-1,-1 1 90,-10-2-1189,-4-10 554</inkml:trace>
@@ -2582,10 +3779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C778B2B-395C-48D4-A69E-65911A94465C}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R34" sqref="R34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2744,10 +3941,18 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" s="11">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>25</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>